<commit_message>
Ajout UTS par jour
</commit_message>
<xml_diff>
--- a/data/raw/Orano-données_2.xlsx
+++ b/data/raw/Orano-données_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dessin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Auteur</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="J4" authorId="0" shapeId="0">
@@ -32,7 +32,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -83,7 +83,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -131,7 +131,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -155,7 +155,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -180,7 +180,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -205,7 +205,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -230,7 +230,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -255,7 +255,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -279,7 +279,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -303,7 +303,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -322,7 +322,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="92">
   <si>
     <t>Commandes</t>
   </si>
@@ -596,15 +596,18 @@
   <si>
     <t>UTS/an</t>
   </si>
+  <si>
+    <t>UTS/jour</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _D_M_-;\-* #,##0.00\ _D_M_-;_-* &quot;-&quot;??\ _D_M_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy\ hh:mm;@"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _D_M_-;\-* #,##0.00\ _D_M_-;_-* &quot;-&quot;??\ _D_M_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy\ hh:mm;@"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
@@ -955,11 +958,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -976,19 +979,19 @@
     <xf numFmtId="2" fontId="7" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1000,16 +1003,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1018,13 +1021,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1033,25 +1036,25 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1063,7 +1066,7 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1071,27 +1074,6 @@
     </xf>
     <xf numFmtId="10" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1147,12 +1129,36 @@
     <xf numFmtId="167" fontId="14" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Milliers_export-SO-2013-03-05 MOSAIC 2013" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pourcentage" xfId="3" builtinId="5"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1170,7 +1176,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1207,7 +1213,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1621,7 +1626,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1738,7 +1742,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3629,7 +3632,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3922,7 +3925,7 @@
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3934,11 +3937,11 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A3:R337"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
@@ -3957,28 +3960,28 @@
   <sheetData>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="D4" s="42" t="s">
+      <c r="B4" s="57"/>
+      <c r="D4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="39" t="s">
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="42" t="s">
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="N4" s="43"/>
-      <c r="O4" s="44"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="61"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -4081,7 +4084,7 @@
       <c r="E7" s="23">
         <v>1</v>
       </c>
-      <c r="F7" s="47">
+      <c r="F7" s="40">
         <v>4.1500000000000002E-2</v>
       </c>
       <c r="G7" s="10">
@@ -4131,7 +4134,7 @@
       <c r="E8" s="23">
         <v>2</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F8" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
       <c r="G8" s="10">
@@ -4182,7 +4185,7 @@
       <c r="E9" s="23">
         <v>3</v>
       </c>
-      <c r="F9" s="47">
+      <c r="F9" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
       <c r="G9" s="10">
@@ -4233,7 +4236,7 @@
       <c r="E10" s="23">
         <v>4</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="40">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="G10" s="10">
@@ -4284,7 +4287,7 @@
       <c r="E11" s="23">
         <v>5</v>
       </c>
-      <c r="F11" s="47">
+      <c r="F11" s="40">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="G11" s="10">
@@ -4335,7 +4338,7 @@
       <c r="E12" s="23">
         <v>6</v>
       </c>
-      <c r="F12" s="47">
+      <c r="F12" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
       <c r="G12" s="10">
@@ -4386,7 +4389,7 @@
       <c r="E13" s="23">
         <v>7</v>
       </c>
-      <c r="F13" s="47">
+      <c r="F13" s="40">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="G13" s="10">
@@ -4437,7 +4440,7 @@
       <c r="E14" s="23">
         <v>8</v>
       </c>
-      <c r="F14" s="47">
+      <c r="F14" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
       <c r="G14" s="10">
@@ -4488,7 +4491,7 @@
       <c r="E15" s="23">
         <v>9</v>
       </c>
-      <c r="F15" s="47">
+      <c r="F15" s="40">
         <v>0.04</v>
       </c>
       <c r="G15" s="10">
@@ -4539,7 +4542,7 @@
       <c r="E16" s="23">
         <v>10</v>
       </c>
-      <c r="F16" s="47">
+      <c r="F16" s="40">
         <v>0.04</v>
       </c>
       <c r="G16" s="10">
@@ -4590,7 +4593,7 @@
       <c r="E17" s="23">
         <v>11</v>
       </c>
-      <c r="F17" s="47">
+      <c r="F17" s="40">
         <v>0.04</v>
       </c>
       <c r="G17" s="10">
@@ -4641,7 +4644,7 @@
       <c r="E18" s="23">
         <v>12</v>
       </c>
-      <c r="F18" s="47">
+      <c r="F18" s="40">
         <v>0.04</v>
       </c>
       <c r="G18" s="10">
@@ -4692,7 +4695,7 @@
       <c r="E19" s="23">
         <v>13</v>
       </c>
-      <c r="F19" s="47">
+      <c r="F19" s="40">
         <v>0.04</v>
       </c>
       <c r="G19" s="10">
@@ -4743,7 +4746,7 @@
       <c r="E20" s="23">
         <v>14</v>
       </c>
-      <c r="F20" s="47">
+      <c r="F20" s="40">
         <v>4.6500000000000007E-2</v>
       </c>
       <c r="G20" s="10">
@@ -4794,7 +4797,7 @@
       <c r="E21" s="23">
         <v>15</v>
       </c>
-      <c r="F21" s="47">
+      <c r="F21" s="40">
         <v>0.04</v>
       </c>
       <c r="G21" s="10">
@@ -4845,7 +4848,7 @@
       <c r="E22" s="23">
         <v>16</v>
       </c>
-      <c r="F22" s="47">
+      <c r="F22" s="40">
         <v>0.04</v>
       </c>
       <c r="G22" s="10">
@@ -4896,7 +4899,7 @@
       <c r="E23" s="23">
         <v>17</v>
       </c>
-      <c r="F23" s="47">
+      <c r="F23" s="40">
         <v>4.9500000000000002E-2</v>
       </c>
       <c r="G23" s="10">
@@ -4947,7 +4950,7 @@
       <c r="E24" s="23">
         <v>18</v>
       </c>
-      <c r="F24" s="47">
+      <c r="F24" s="40">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="G24" s="10">
@@ -4998,7 +5001,7 @@
       <c r="E25" s="23">
         <v>19</v>
       </c>
-      <c r="F25" s="47">
+      <c r="F25" s="40">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="G25" s="10">
@@ -5049,7 +5052,7 @@
       <c r="E26" s="23">
         <v>20</v>
       </c>
-      <c r="F26" s="47">
+      <c r="F26" s="40">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="G26" s="10">
@@ -5100,7 +5103,7 @@
       <c r="E27" s="23">
         <v>21</v>
       </c>
-      <c r="F27" s="47">
+      <c r="F27" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
       <c r="G27" s="10">
@@ -5151,7 +5154,7 @@
       <c r="E28" s="23">
         <v>22</v>
       </c>
-      <c r="F28" s="47">
+      <c r="F28" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
       <c r="G28" s="10">
@@ -5202,7 +5205,7 @@
       <c r="E29" s="23">
         <v>23</v>
       </c>
-      <c r="F29" s="47">
+      <c r="F29" s="40">
         <v>0.04</v>
       </c>
       <c r="G29" s="10">
@@ -5253,7 +5256,7 @@
       <c r="E30" s="23">
         <v>24</v>
       </c>
-      <c r="F30" s="47">
+      <c r="F30" s="40">
         <v>0.04</v>
       </c>
       <c r="G30" s="10">
@@ -5304,7 +5307,7 @@
       <c r="E31" s="23">
         <v>25</v>
       </c>
-      <c r="F31" s="47">
+      <c r="F31" s="40">
         <v>0.04</v>
       </c>
       <c r="G31" s="10">
@@ -5355,7 +5358,7 @@
       <c r="E32" s="23">
         <v>26</v>
       </c>
-      <c r="F32" s="47">
+      <c r="F32" s="40">
         <v>0.04</v>
       </c>
       <c r="G32" s="10">
@@ -5406,7 +5409,7 @@
       <c r="E33" s="23">
         <v>27</v>
       </c>
-      <c r="F33" s="47">
+      <c r="F33" s="40">
         <v>0.04</v>
       </c>
       <c r="G33" s="10">
@@ -5457,7 +5460,7 @@
       <c r="E34" s="23">
         <v>28</v>
       </c>
-      <c r="F34" s="47">
+      <c r="F34" s="40">
         <v>0.04</v>
       </c>
       <c r="G34" s="10">
@@ -5508,7 +5511,7 @@
       <c r="E35" s="23">
         <v>29</v>
       </c>
-      <c r="F35" s="47">
+      <c r="F35" s="40">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="G35" s="10">
@@ -5559,7 +5562,7 @@
       <c r="E36" s="23">
         <v>30</v>
       </c>
-      <c r="F36" s="47">
+      <c r="F36" s="40">
         <v>4.6699999999999998E-2</v>
       </c>
       <c r="G36" s="10">
@@ -5610,7 +5613,7 @@
       <c r="E37" s="23">
         <v>31</v>
       </c>
-      <c r="F37" s="47">
+      <c r="F37" s="40">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="G37" s="10">
@@ -5661,7 +5664,7 @@
       <c r="E38" s="23">
         <v>32</v>
       </c>
-      <c r="F38" s="47">
+      <c r="F38" s="40">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="G38" s="10">
@@ -5712,7 +5715,7 @@
       <c r="E39" s="23">
         <v>33</v>
       </c>
-      <c r="F39" s="47">
+      <c r="F39" s="40">
         <v>0.04</v>
       </c>
       <c r="G39" s="10">
@@ -5763,7 +5766,7 @@
       <c r="E40" s="23">
         <v>34</v>
       </c>
-      <c r="F40" s="47">
+      <c r="F40" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
       <c r="G40" s="10">
@@ -5814,7 +5817,7 @@
       <c r="E41" s="23">
         <v>35</v>
       </c>
-      <c r="F41" s="47">
+      <c r="F41" s="40">
         <v>4.4000000000000004E-2</v>
       </c>
       <c r="G41" s="10">
@@ -5865,7 +5868,7 @@
       <c r="E42" s="23">
         <v>36</v>
       </c>
-      <c r="F42" s="47">
+      <c r="F42" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
       <c r="G42" s="10">
@@ -5916,7 +5919,7 @@
       <c r="E43" s="23">
         <v>37</v>
       </c>
-      <c r="F43" s="47">
+      <c r="F43" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
       <c r="G43" s="10">
@@ -5967,7 +5970,7 @@
       <c r="E44" s="23">
         <v>38</v>
       </c>
-      <c r="F44" s="47">
+      <c r="F44" s="40">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="G44" s="10">
@@ -6018,7 +6021,7 @@
       <c r="E45" s="23">
         <v>39</v>
       </c>
-      <c r="F45" s="47">
+      <c r="F45" s="40">
         <v>4.3700000000000003E-2</v>
       </c>
       <c r="G45" s="10">
@@ -6069,7 +6072,7 @@
       <c r="E46" s="23">
         <v>40</v>
       </c>
-      <c r="F46" s="47">
+      <c r="F46" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
       <c r="G46" s="10">
@@ -6120,7 +6123,7 @@
       <c r="E47" s="23">
         <v>41</v>
       </c>
-      <c r="F47" s="47">
+      <c r="F47" s="40">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="G47" s="10">
@@ -6171,7 +6174,7 @@
       <c r="E48" s="23">
         <v>42</v>
       </c>
-      <c r="F48" s="47">
+      <c r="F48" s="40">
         <v>4.4000000000000004E-2</v>
       </c>
       <c r="G48" s="10">
@@ -6222,7 +6225,7 @@
       <c r="E49" s="23">
         <v>43</v>
       </c>
-      <c r="F49" s="47">
+      <c r="F49" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
       <c r="G49" s="10">
@@ -6273,7 +6276,7 @@
       <c r="E50" s="23">
         <v>44</v>
       </c>
-      <c r="F50" s="47">
+      <c r="F50" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
       <c r="G50" s="10">
@@ -6324,7 +6327,7 @@
       <c r="E51" s="23">
         <v>45</v>
       </c>
-      <c r="F51" s="47">
+      <c r="F51" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
       <c r="G51" s="10">
@@ -6375,7 +6378,7 @@
       <c r="E52" s="23">
         <v>46</v>
       </c>
-      <c r="F52" s="47">
+      <c r="F52" s="40">
         <v>4.4000000000000004E-2</v>
       </c>
       <c r="G52" s="10">
@@ -6426,7 +6429,7 @@
       <c r="E53" s="24">
         <v>47</v>
       </c>
-      <c r="F53" s="48">
+      <c r="F53" s="41">
         <v>4.4000000000000004E-2</v>
       </c>
       <c r="G53" s="25">
@@ -6471,7 +6474,7 @@
       <c r="B54" s="28">
         <v>45627</v>
       </c>
-      <c r="F54" s="46"/>
+      <c r="F54" s="39"/>
       <c r="Q54" s="38"/>
       <c r="R54" s="38"/>
     </row>
@@ -6482,7 +6485,7 @@
       <c r="B55" s="28">
         <v>45658</v>
       </c>
-      <c r="F55" s="46"/>
+      <c r="F55" s="39"/>
       <c r="Q55" s="38"/>
       <c r="R55" s="38"/>
     </row>
@@ -6493,7 +6496,7 @@
       <c r="B56" s="28">
         <v>45689</v>
       </c>
-      <c r="F56" s="46"/>
+      <c r="F56" s="39"/>
       <c r="Q56" s="38"/>
       <c r="R56" s="38"/>
     </row>
@@ -6504,7 +6507,7 @@
       <c r="B57" s="28">
         <v>45717</v>
       </c>
-      <c r="F57" s="46"/>
+      <c r="F57" s="39"/>
       <c r="Q57" s="38"/>
       <c r="R57" s="38"/>
     </row>
@@ -6515,7 +6518,7 @@
       <c r="B58" s="28">
         <v>45748</v>
       </c>
-      <c r="F58" s="46"/>
+      <c r="F58" s="39"/>
       <c r="Q58" s="38"/>
       <c r="R58" s="38"/>
     </row>
@@ -6526,7 +6529,7 @@
       <c r="B59" s="28">
         <v>45778</v>
       </c>
-      <c r="F59" s="46"/>
+      <c r="F59" s="39"/>
       <c r="Q59" s="38"/>
       <c r="R59" s="38"/>
     </row>
@@ -6537,7 +6540,7 @@
       <c r="B60" s="28">
         <v>45809</v>
       </c>
-      <c r="F60" s="46"/>
+      <c r="F60" s="39"/>
       <c r="Q60" s="38"/>
       <c r="R60" s="38"/>
     </row>
@@ -6548,7 +6551,7 @@
       <c r="B61" s="28">
         <v>45839</v>
       </c>
-      <c r="F61" s="46"/>
+      <c r="F61" s="39"/>
       <c r="Q61" s="38"/>
       <c r="R61" s="38"/>
     </row>
@@ -6559,7 +6562,7 @@
       <c r="B62" s="28">
         <v>45870</v>
       </c>
-      <c r="F62" s="46"/>
+      <c r="F62" s="39"/>
       <c r="Q62" s="38"/>
       <c r="R62" s="38"/>
     </row>
@@ -6570,7 +6573,7 @@
       <c r="B63" s="28">
         <v>45901</v>
       </c>
-      <c r="F63" s="46"/>
+      <c r="F63" s="39"/>
       <c r="Q63" s="38"/>
       <c r="R63" s="38"/>
     </row>
@@ -6581,7 +6584,7 @@
       <c r="B64" s="28">
         <v>45931</v>
       </c>
-      <c r="F64" s="46"/>
+      <c r="F64" s="39"/>
       <c r="Q64" s="38"/>
       <c r="R64" s="38"/>
     </row>
@@ -6592,7 +6595,7 @@
       <c r="B65" s="28">
         <v>45962</v>
       </c>
-      <c r="F65" s="46"/>
+      <c r="F65" s="39"/>
       <c r="Q65" s="38"/>
       <c r="R65" s="38"/>
     </row>
@@ -6603,7 +6606,7 @@
       <c r="B66" s="28">
         <v>45992</v>
       </c>
-      <c r="F66" s="46"/>
+      <c r="F66" s="39"/>
       <c r="Q66" s="38"/>
       <c r="R66" s="38"/>
     </row>
@@ -6614,7 +6617,7 @@
       <c r="B67" s="28">
         <v>46023</v>
       </c>
-      <c r="F67" s="46"/>
+      <c r="F67" s="39"/>
       <c r="Q67" s="38"/>
       <c r="R67" s="38"/>
     </row>
@@ -6625,7 +6628,7 @@
       <c r="B68" s="28">
         <v>46054</v>
       </c>
-      <c r="F68" s="46"/>
+      <c r="F68" s="39"/>
       <c r="Q68" s="38"/>
       <c r="R68" s="38"/>
     </row>
@@ -6636,7 +6639,7 @@
       <c r="B69" s="28">
         <v>46082</v>
       </c>
-      <c r="F69" s="46"/>
+      <c r="F69" s="39"/>
       <c r="Q69" s="38"/>
       <c r="R69" s="38"/>
     </row>
@@ -6647,7 +6650,7 @@
       <c r="B70" s="28">
         <v>46113</v>
       </c>
-      <c r="F70" s="46"/>
+      <c r="F70" s="39"/>
       <c r="Q70" s="38"/>
       <c r="R70" s="38"/>
     </row>
@@ -6658,7 +6661,7 @@
       <c r="B71" s="28">
         <v>46143</v>
       </c>
-      <c r="F71" s="46"/>
+      <c r="F71" s="39"/>
       <c r="Q71" s="38"/>
       <c r="R71" s="38"/>
     </row>
@@ -6669,7 +6672,7 @@
       <c r="B72" s="28">
         <v>46174</v>
       </c>
-      <c r="F72" s="46"/>
+      <c r="F72" s="39"/>
       <c r="Q72" s="38"/>
       <c r="R72" s="38"/>
     </row>
@@ -6680,7 +6683,7 @@
       <c r="B73" s="28">
         <v>46204</v>
       </c>
-      <c r="F73" s="46"/>
+      <c r="F73" s="39"/>
       <c r="Q73" s="38"/>
       <c r="R73" s="38"/>
     </row>
@@ -6691,7 +6694,7 @@
       <c r="B74" s="28">
         <v>46235</v>
       </c>
-      <c r="F74" s="46"/>
+      <c r="F74" s="39"/>
       <c r="Q74" s="38"/>
       <c r="R74" s="38"/>
     </row>
@@ -6702,7 +6705,7 @@
       <c r="B75" s="28">
         <v>46266</v>
       </c>
-      <c r="F75" s="46"/>
+      <c r="F75" s="39"/>
       <c r="Q75" s="38"/>
       <c r="R75" s="38"/>
     </row>
@@ -6713,7 +6716,7 @@
       <c r="B76" s="28">
         <v>46296</v>
       </c>
-      <c r="F76" s="46"/>
+      <c r="F76" s="39"/>
       <c r="Q76" s="38"/>
       <c r="R76" s="38"/>
     </row>
@@ -6724,7 +6727,7 @@
       <c r="B77" s="28">
         <v>46327</v>
       </c>
-      <c r="F77" s="46"/>
+      <c r="F77" s="39"/>
       <c r="Q77" s="38"/>
       <c r="R77" s="38"/>
     </row>
@@ -6735,7 +6738,7 @@
       <c r="B78" s="28">
         <v>46357</v>
       </c>
-      <c r="F78" s="46"/>
+      <c r="F78" s="39"/>
       <c r="Q78" s="38"/>
       <c r="R78" s="38"/>
     </row>
@@ -6746,7 +6749,7 @@
       <c r="B79" s="28">
         <v>46388</v>
       </c>
-      <c r="F79" s="46"/>
+      <c r="F79" s="39"/>
       <c r="Q79" s="38"/>
       <c r="R79" s="38"/>
     </row>
@@ -6757,7 +6760,7 @@
       <c r="B80" s="28">
         <v>46419</v>
       </c>
-      <c r="F80" s="46"/>
+      <c r="F80" s="39"/>
       <c r="Q80" s="38"/>
       <c r="R80" s="38"/>
     </row>
@@ -6768,7 +6771,7 @@
       <c r="B81" s="28">
         <v>46447</v>
       </c>
-      <c r="F81" s="46"/>
+      <c r="F81" s="39"/>
       <c r="Q81" s="38"/>
       <c r="R81" s="38"/>
     </row>
@@ -6779,7 +6782,7 @@
       <c r="B82" s="28">
         <v>46478</v>
       </c>
-      <c r="F82" s="46"/>
+      <c r="F82" s="39"/>
       <c r="Q82" s="38"/>
       <c r="R82" s="38"/>
     </row>
@@ -6790,7 +6793,7 @@
       <c r="B83" s="28">
         <v>46508</v>
       </c>
-      <c r="F83" s="46"/>
+      <c r="F83" s="39"/>
       <c r="Q83" s="38"/>
       <c r="R83" s="38"/>
     </row>
@@ -6801,7 +6804,7 @@
       <c r="B84" s="28">
         <v>46539</v>
       </c>
-      <c r="F84" s="46"/>
+      <c r="F84" s="39"/>
       <c r="Q84" s="38"/>
       <c r="R84" s="38"/>
     </row>
@@ -6812,7 +6815,7 @@
       <c r="B85" s="28">
         <v>46569</v>
       </c>
-      <c r="F85" s="46"/>
+      <c r="F85" s="39"/>
       <c r="Q85" s="38"/>
       <c r="R85" s="38"/>
     </row>
@@ -6823,7 +6826,7 @@
       <c r="B86" s="28">
         <v>46600</v>
       </c>
-      <c r="F86" s="46"/>
+      <c r="F86" s="39"/>
       <c r="Q86" s="38"/>
       <c r="R86" s="38"/>
     </row>
@@ -6834,7 +6837,7 @@
       <c r="B87" s="28">
         <v>46631</v>
       </c>
-      <c r="F87" s="46"/>
+      <c r="F87" s="39"/>
       <c r="Q87" s="38"/>
       <c r="R87" s="38"/>
     </row>
@@ -6845,7 +6848,7 @@
       <c r="B88" s="28">
         <v>46661</v>
       </c>
-      <c r="F88" s="46"/>
+      <c r="F88" s="39"/>
       <c r="Q88" s="38"/>
       <c r="R88" s="38"/>
     </row>
@@ -6856,7 +6859,7 @@
       <c r="B89" s="28">
         <v>46692</v>
       </c>
-      <c r="F89" s="46"/>
+      <c r="F89" s="39"/>
       <c r="Q89" s="38"/>
       <c r="R89" s="38"/>
     </row>
@@ -6867,7 +6870,7 @@
       <c r="B90" s="28">
         <v>46722</v>
       </c>
-      <c r="F90" s="46"/>
+      <c r="F90" s="39"/>
       <c r="Q90" s="38"/>
       <c r="R90" s="38"/>
     </row>
@@ -6878,7 +6881,7 @@
       <c r="B91" s="28">
         <v>46753</v>
       </c>
-      <c r="F91" s="46"/>
+      <c r="F91" s="39"/>
       <c r="Q91" s="38"/>
       <c r="R91" s="38"/>
     </row>
@@ -6889,7 +6892,7 @@
       <c r="B92" s="28">
         <v>46784</v>
       </c>
-      <c r="F92" s="46"/>
+      <c r="F92" s="39"/>
       <c r="Q92" s="38"/>
       <c r="R92" s="38"/>
     </row>
@@ -6900,7 +6903,7 @@
       <c r="B93" s="28">
         <v>46813</v>
       </c>
-      <c r="F93" s="46"/>
+      <c r="F93" s="39"/>
       <c r="Q93" s="38"/>
       <c r="R93" s="38"/>
     </row>
@@ -6911,7 +6914,7 @@
       <c r="B94" s="28">
         <v>46844</v>
       </c>
-      <c r="F94" s="46"/>
+      <c r="F94" s="39"/>
       <c r="Q94" s="38"/>
       <c r="R94" s="38"/>
     </row>
@@ -6922,7 +6925,7 @@
       <c r="B95" s="28">
         <v>46874</v>
       </c>
-      <c r="F95" s="46"/>
+      <c r="F95" s="39"/>
       <c r="Q95" s="38"/>
       <c r="R95" s="38"/>
     </row>
@@ -6933,7 +6936,7 @@
       <c r="B96" s="28">
         <v>46905</v>
       </c>
-      <c r="F96" s="46"/>
+      <c r="F96" s="39"/>
       <c r="Q96" s="38"/>
       <c r="R96" s="38"/>
     </row>
@@ -6944,7 +6947,7 @@
       <c r="B97" s="28">
         <v>46935</v>
       </c>
-      <c r="F97" s="46"/>
+      <c r="F97" s="39"/>
       <c r="Q97" s="38"/>
       <c r="R97" s="38"/>
     </row>
@@ -6955,7 +6958,7 @@
       <c r="B98" s="28">
         <v>46966</v>
       </c>
-      <c r="F98" s="46"/>
+      <c r="F98" s="39"/>
       <c r="Q98" s="38"/>
       <c r="R98" s="38"/>
     </row>
@@ -6966,7 +6969,7 @@
       <c r="B99" s="28">
         <v>46997</v>
       </c>
-      <c r="F99" s="46"/>
+      <c r="F99" s="39"/>
       <c r="Q99" s="38"/>
       <c r="R99" s="38"/>
     </row>
@@ -6977,7 +6980,7 @@
       <c r="B100" s="28">
         <v>47027</v>
       </c>
-      <c r="F100" s="46"/>
+      <c r="F100" s="39"/>
       <c r="Q100" s="38"/>
       <c r="R100" s="38"/>
     </row>
@@ -6988,7 +6991,7 @@
       <c r="B101" s="28">
         <v>47058</v>
       </c>
-      <c r="F101" s="46"/>
+      <c r="F101" s="39"/>
       <c r="Q101" s="38"/>
       <c r="R101" s="38"/>
     </row>
@@ -6999,7 +7002,7 @@
       <c r="B102" s="28">
         <v>47088</v>
       </c>
-      <c r="F102" s="46"/>
+      <c r="F102" s="39"/>
       <c r="Q102" s="38"/>
       <c r="R102" s="38"/>
     </row>
@@ -7010,7 +7013,7 @@
       <c r="B103" s="28">
         <v>47119</v>
       </c>
-      <c r="F103" s="46"/>
+      <c r="F103" s="39"/>
       <c r="Q103" s="38"/>
       <c r="R103" s="38"/>
     </row>
@@ -7021,7 +7024,7 @@
       <c r="B104" s="28">
         <v>47150</v>
       </c>
-      <c r="F104" s="46"/>
+      <c r="F104" s="39"/>
       <c r="Q104" s="38"/>
       <c r="R104" s="38"/>
     </row>
@@ -7032,7 +7035,7 @@
       <c r="B105" s="28">
         <v>47178</v>
       </c>
-      <c r="F105" s="46"/>
+      <c r="F105" s="39"/>
       <c r="Q105" s="38"/>
       <c r="R105" s="38"/>
     </row>
@@ -7043,7 +7046,7 @@
       <c r="B106" s="28">
         <v>47209</v>
       </c>
-      <c r="F106" s="46"/>
+      <c r="F106" s="39"/>
       <c r="Q106" s="38"/>
       <c r="R106" s="38"/>
     </row>
@@ -7054,7 +7057,7 @@
       <c r="B107" s="28">
         <v>47239</v>
       </c>
-      <c r="F107" s="46"/>
+      <c r="F107" s="39"/>
       <c r="Q107" s="38"/>
       <c r="R107" s="38"/>
     </row>
@@ -7065,7 +7068,7 @@
       <c r="B108" s="28">
         <v>47270</v>
       </c>
-      <c r="F108" s="46"/>
+      <c r="F108" s="39"/>
       <c r="Q108" s="38"/>
       <c r="R108" s="38"/>
     </row>
@@ -7076,7 +7079,7 @@
       <c r="B109" s="28">
         <v>47300</v>
       </c>
-      <c r="F109" s="46"/>
+      <c r="F109" s="39"/>
       <c r="Q109" s="38"/>
       <c r="R109" s="38"/>
     </row>
@@ -7087,7 +7090,7 @@
       <c r="B110" s="28">
         <v>47331</v>
       </c>
-      <c r="F110" s="46"/>
+      <c r="F110" s="39"/>
       <c r="Q110" s="38"/>
       <c r="R110" s="38"/>
     </row>
@@ -7098,7 +7101,7 @@
       <c r="B111" s="28">
         <v>47362</v>
       </c>
-      <c r="F111" s="46"/>
+      <c r="F111" s="39"/>
       <c r="Q111" s="38"/>
       <c r="R111" s="38"/>
     </row>
@@ -7109,7 +7112,7 @@
       <c r="B112" s="28">
         <v>47392</v>
       </c>
-      <c r="F112" s="46"/>
+      <c r="F112" s="39"/>
       <c r="Q112" s="38"/>
       <c r="R112" s="38"/>
     </row>
@@ -7120,7 +7123,7 @@
       <c r="B113" s="28">
         <v>47423</v>
       </c>
-      <c r="F113" s="46"/>
+      <c r="F113" s="39"/>
       <c r="Q113" s="38"/>
       <c r="R113" s="38"/>
     </row>
@@ -7131,7 +7134,7 @@
       <c r="B114" s="28">
         <v>47453</v>
       </c>
-      <c r="F114" s="46"/>
+      <c r="F114" s="39"/>
       <c r="Q114" s="38"/>
       <c r="R114" s="38"/>
     </row>
@@ -7142,7 +7145,7 @@
       <c r="B115" s="28">
         <v>47484</v>
       </c>
-      <c r="F115" s="46"/>
+      <c r="F115" s="39"/>
       <c r="Q115" s="38"/>
       <c r="R115" s="38"/>
     </row>
@@ -7153,7 +7156,7 @@
       <c r="B116" s="28">
         <v>47515</v>
       </c>
-      <c r="F116" s="46"/>
+      <c r="F116" s="39"/>
       <c r="Q116" s="38"/>
       <c r="R116" s="38"/>
     </row>
@@ -7164,7 +7167,7 @@
       <c r="B117" s="28">
         <v>47543</v>
       </c>
-      <c r="F117" s="46"/>
+      <c r="F117" s="39"/>
       <c r="Q117" s="38"/>
       <c r="R117" s="38"/>
     </row>
@@ -7175,7 +7178,7 @@
       <c r="B118" s="28">
         <v>47574</v>
       </c>
-      <c r="F118" s="46"/>
+      <c r="F118" s="39"/>
       <c r="Q118" s="38"/>
       <c r="R118" s="38"/>
     </row>
@@ -7186,7 +7189,7 @@
       <c r="B119" s="28">
         <v>47604</v>
       </c>
-      <c r="F119" s="46"/>
+      <c r="F119" s="39"/>
       <c r="Q119" s="38"/>
       <c r="R119" s="38"/>
     </row>
@@ -7197,7 +7200,7 @@
       <c r="B120" s="28">
         <v>47635</v>
       </c>
-      <c r="F120" s="46"/>
+      <c r="F120" s="39"/>
       <c r="Q120" s="38"/>
       <c r="R120" s="38"/>
     </row>
@@ -7208,7 +7211,7 @@
       <c r="B121" s="28">
         <v>47665</v>
       </c>
-      <c r="F121" s="46"/>
+      <c r="F121" s="39"/>
       <c r="Q121" s="38"/>
       <c r="R121" s="38"/>
     </row>
@@ -7219,7 +7222,7 @@
       <c r="B122" s="28">
         <v>47696</v>
       </c>
-      <c r="F122" s="46"/>
+      <c r="F122" s="39"/>
       <c r="Q122" s="38"/>
       <c r="R122" s="38"/>
     </row>
@@ -7230,7 +7233,7 @@
       <c r="B123" s="28">
         <v>47727</v>
       </c>
-      <c r="F123" s="46"/>
+      <c r="F123" s="39"/>
       <c r="Q123" s="38"/>
       <c r="R123" s="38"/>
     </row>
@@ -7241,7 +7244,7 @@
       <c r="B124" s="28">
         <v>47757</v>
       </c>
-      <c r="F124" s="46"/>
+      <c r="F124" s="39"/>
       <c r="Q124" s="38"/>
       <c r="R124" s="38"/>
     </row>
@@ -7252,7 +7255,7 @@
       <c r="B125" s="28">
         <v>47788</v>
       </c>
-      <c r="F125" s="46"/>
+      <c r="F125" s="39"/>
       <c r="Q125" s="38"/>
       <c r="R125" s="38"/>
     </row>
@@ -7263,7 +7266,7 @@
       <c r="B126" s="28">
         <v>47818</v>
       </c>
-      <c r="F126" s="46"/>
+      <c r="F126" s="39"/>
       <c r="Q126" s="38"/>
       <c r="R126" s="38"/>
     </row>
@@ -7274,7 +7277,7 @@
       <c r="B127" s="28">
         <v>47849</v>
       </c>
-      <c r="F127" s="46"/>
+      <c r="F127" s="39"/>
       <c r="Q127" s="38"/>
       <c r="R127" s="38"/>
     </row>
@@ -7285,7 +7288,7 @@
       <c r="B128" s="28">
         <v>47880</v>
       </c>
-      <c r="F128" s="46"/>
+      <c r="F128" s="39"/>
       <c r="Q128" s="38"/>
       <c r="R128" s="38"/>
     </row>
@@ -7296,7 +7299,7 @@
       <c r="B129" s="28">
         <v>47908</v>
       </c>
-      <c r="F129" s="46"/>
+      <c r="F129" s="39"/>
       <c r="Q129" s="38"/>
       <c r="R129" s="38"/>
     </row>
@@ -7307,7 +7310,7 @@
       <c r="B130" s="28">
         <v>47939</v>
       </c>
-      <c r="F130" s="46"/>
+      <c r="F130" s="39"/>
       <c r="Q130" s="38"/>
       <c r="R130" s="38"/>
     </row>
@@ -7318,7 +7321,7 @@
       <c r="B131" s="28">
         <v>47969</v>
       </c>
-      <c r="F131" s="46"/>
+      <c r="F131" s="39"/>
       <c r="Q131" s="38"/>
       <c r="R131" s="38"/>
     </row>
@@ -7329,7 +7332,7 @@
       <c r="B132" s="28">
         <v>48000</v>
       </c>
-      <c r="F132" s="46"/>
+      <c r="F132" s="39"/>
       <c r="Q132" s="38"/>
       <c r="R132" s="38"/>
     </row>
@@ -7340,7 +7343,7 @@
       <c r="B133" s="28">
         <v>48030</v>
       </c>
-      <c r="F133" s="46"/>
+      <c r="F133" s="39"/>
       <c r="Q133" s="38"/>
       <c r="R133" s="38"/>
     </row>
@@ -7351,7 +7354,7 @@
       <c r="B134" s="28">
         <v>48061</v>
       </c>
-      <c r="F134" s="46"/>
+      <c r="F134" s="39"/>
       <c r="Q134" s="38"/>
       <c r="R134" s="38"/>
     </row>
@@ -7362,7 +7365,7 @@
       <c r="B135" s="28">
         <v>48092</v>
       </c>
-      <c r="F135" s="46"/>
+      <c r="F135" s="39"/>
       <c r="Q135" s="38"/>
       <c r="R135" s="38"/>
     </row>
@@ -7373,7 +7376,7 @@
       <c r="B136" s="28">
         <v>48122</v>
       </c>
-      <c r="F136" s="46"/>
+      <c r="F136" s="39"/>
       <c r="Q136" s="38"/>
       <c r="R136" s="38"/>
     </row>
@@ -7384,7 +7387,7 @@
       <c r="B137" s="28">
         <v>48153</v>
       </c>
-      <c r="F137" s="46"/>
+      <c r="F137" s="39"/>
       <c r="Q137" s="38"/>
       <c r="R137" s="38"/>
     </row>
@@ -7395,7 +7398,7 @@
       <c r="B138" s="28">
         <v>48183</v>
       </c>
-      <c r="F138" s="46"/>
+      <c r="F138" s="39"/>
       <c r="Q138" s="38"/>
       <c r="R138" s="38"/>
     </row>
@@ -7406,7 +7409,7 @@
       <c r="B139" s="28">
         <v>48214</v>
       </c>
-      <c r="F139" s="46"/>
+      <c r="F139" s="39"/>
       <c r="Q139" s="38"/>
       <c r="R139" s="38"/>
     </row>
@@ -7417,7 +7420,7 @@
       <c r="B140" s="28">
         <v>48245</v>
       </c>
-      <c r="F140" s="46"/>
+      <c r="F140" s="39"/>
       <c r="Q140" s="38"/>
       <c r="R140" s="38"/>
     </row>
@@ -7428,7 +7431,7 @@
       <c r="B141" s="28">
         <v>48274</v>
       </c>
-      <c r="F141" s="46"/>
+      <c r="F141" s="39"/>
       <c r="Q141" s="38"/>
       <c r="R141" s="38"/>
     </row>
@@ -7439,7 +7442,7 @@
       <c r="B142" s="28">
         <v>48305</v>
       </c>
-      <c r="F142" s="46"/>
+      <c r="F142" s="39"/>
       <c r="Q142" s="38"/>
       <c r="R142" s="38"/>
     </row>
@@ -7450,7 +7453,7 @@
       <c r="B143" s="28">
         <v>48335</v>
       </c>
-      <c r="F143" s="46"/>
+      <c r="F143" s="39"/>
       <c r="Q143" s="38"/>
       <c r="R143" s="38"/>
     </row>
@@ -7461,7 +7464,7 @@
       <c r="B144" s="28">
         <v>48366</v>
       </c>
-      <c r="F144" s="46"/>
+      <c r="F144" s="39"/>
       <c r="Q144" s="38"/>
       <c r="R144" s="38"/>
     </row>
@@ -7472,7 +7475,7 @@
       <c r="B145" s="28">
         <v>48396</v>
       </c>
-      <c r="F145" s="46"/>
+      <c r="F145" s="39"/>
       <c r="Q145" s="38"/>
       <c r="R145" s="38"/>
     </row>
@@ -7483,7 +7486,7 @@
       <c r="B146" s="28">
         <v>48427</v>
       </c>
-      <c r="F146" s="46"/>
+      <c r="F146" s="39"/>
       <c r="Q146" s="38"/>
       <c r="R146" s="38"/>
     </row>
@@ -7494,7 +7497,7 @@
       <c r="B147" s="28">
         <v>48458</v>
       </c>
-      <c r="F147" s="46"/>
+      <c r="F147" s="39"/>
       <c r="Q147" s="38"/>
       <c r="R147" s="38"/>
     </row>
@@ -7505,7 +7508,7 @@
       <c r="B148" s="28">
         <v>48488</v>
       </c>
-      <c r="F148" s="46"/>
+      <c r="F148" s="39"/>
       <c r="Q148" s="38"/>
       <c r="R148" s="38"/>
     </row>
@@ -7516,942 +7519,942 @@
       <c r="B149" s="29">
         <v>48519</v>
       </c>
-      <c r="F149" s="46"/>
+      <c r="F149" s="39"/>
       <c r="Q149" s="38"/>
       <c r="R149" s="38"/>
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F150" s="46"/>
+      <c r="F150" s="39"/>
       <c r="Q150" s="38"/>
       <c r="R150" s="38"/>
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F151" s="46"/>
+      <c r="F151" s="39"/>
       <c r="Q151" s="38"/>
       <c r="R151" s="38"/>
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F152" s="46"/>
+      <c r="F152" s="39"/>
       <c r="Q152" s="38"/>
       <c r="R152" s="38"/>
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F153" s="46"/>
+      <c r="F153" s="39"/>
       <c r="Q153" s="38"/>
       <c r="R153" s="38"/>
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F154" s="46"/>
+      <c r="F154" s="39"/>
       <c r="Q154" s="38"/>
       <c r="R154" s="38"/>
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F155" s="46"/>
+      <c r="F155" s="39"/>
       <c r="Q155" s="38"/>
       <c r="R155" s="38"/>
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F156" s="46"/>
+      <c r="F156" s="39"/>
       <c r="Q156" s="38"/>
       <c r="R156" s="38"/>
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F157" s="46"/>
+      <c r="F157" s="39"/>
       <c r="Q157" s="38"/>
       <c r="R157" s="38"/>
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F158" s="46"/>
+      <c r="F158" s="39"/>
       <c r="Q158" s="38"/>
       <c r="R158" s="38"/>
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F159" s="46"/>
+      <c r="F159" s="39"/>
       <c r="Q159" s="38"/>
       <c r="R159" s="38"/>
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F160" s="46"/>
+      <c r="F160" s="39"/>
       <c r="Q160" s="38"/>
       <c r="R160" s="38"/>
     </row>
     <row r="161" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F161" s="46"/>
+      <c r="F161" s="39"/>
       <c r="Q161" s="38"/>
       <c r="R161" s="38"/>
     </row>
     <row r="162" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F162" s="46"/>
+      <c r="F162" s="39"/>
       <c r="Q162" s="38"/>
       <c r="R162" s="38"/>
     </row>
     <row r="163" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F163" s="46"/>
+      <c r="F163" s="39"/>
       <c r="Q163" s="38"/>
       <c r="R163" s="38"/>
     </row>
     <row r="164" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F164" s="46"/>
+      <c r="F164" s="39"/>
       <c r="Q164" s="38"/>
       <c r="R164" s="38"/>
     </row>
     <row r="165" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F165" s="46"/>
+      <c r="F165" s="39"/>
       <c r="Q165" s="38"/>
       <c r="R165" s="38"/>
     </row>
     <row r="166" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F166" s="46"/>
+      <c r="F166" s="39"/>
       <c r="Q166" s="38"/>
       <c r="R166" s="38"/>
     </row>
     <row r="167" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F167" s="46"/>
+      <c r="F167" s="39"/>
       <c r="Q167" s="38"/>
       <c r="R167" s="38"/>
     </row>
     <row r="168" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F168" s="46"/>
+      <c r="F168" s="39"/>
       <c r="Q168" s="38"/>
       <c r="R168" s="38"/>
     </row>
     <row r="169" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F169" s="46"/>
+      <c r="F169" s="39"/>
       <c r="Q169" s="38"/>
       <c r="R169" s="38"/>
     </row>
     <row r="170" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F170" s="46"/>
+      <c r="F170" s="39"/>
       <c r="Q170" s="38"/>
       <c r="R170" s="38"/>
     </row>
     <row r="171" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F171" s="46"/>
+      <c r="F171" s="39"/>
       <c r="Q171" s="38"/>
       <c r="R171" s="38"/>
     </row>
     <row r="172" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F172" s="46"/>
+      <c r="F172" s="39"/>
       <c r="Q172" s="38"/>
       <c r="R172" s="38"/>
     </row>
     <row r="173" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F173" s="46"/>
+      <c r="F173" s="39"/>
       <c r="Q173" s="38"/>
       <c r="R173" s="38"/>
     </row>
     <row r="174" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F174" s="46"/>
+      <c r="F174" s="39"/>
       <c r="Q174" s="38"/>
       <c r="R174" s="38"/>
     </row>
     <row r="175" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F175" s="46"/>
+      <c r="F175" s="39"/>
       <c r="Q175" s="38"/>
       <c r="R175" s="38"/>
     </row>
     <row r="176" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F176" s="46"/>
+      <c r="F176" s="39"/>
       <c r="Q176" s="38"/>
       <c r="R176" s="38"/>
     </row>
     <row r="177" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F177" s="46"/>
+      <c r="F177" s="39"/>
       <c r="Q177" s="38"/>
       <c r="R177" s="38"/>
     </row>
     <row r="178" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F178" s="46"/>
+      <c r="F178" s="39"/>
       <c r="Q178" s="38"/>
       <c r="R178" s="38"/>
     </row>
     <row r="179" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F179" s="46"/>
+      <c r="F179" s="39"/>
       <c r="Q179" s="38"/>
       <c r="R179" s="38"/>
     </row>
     <row r="180" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F180" s="46"/>
+      <c r="F180" s="39"/>
       <c r="Q180" s="38"/>
       <c r="R180" s="38"/>
     </row>
     <row r="181" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F181" s="46"/>
+      <c r="F181" s="39"/>
       <c r="Q181" s="38"/>
       <c r="R181" s="38"/>
     </row>
     <row r="182" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F182" s="46"/>
+      <c r="F182" s="39"/>
       <c r="Q182" s="38"/>
       <c r="R182" s="38"/>
     </row>
     <row r="183" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F183" s="46"/>
+      <c r="F183" s="39"/>
       <c r="Q183" s="38"/>
       <c r="R183" s="38"/>
     </row>
     <row r="184" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F184" s="46"/>
+      <c r="F184" s="39"/>
       <c r="Q184" s="38"/>
       <c r="R184" s="38"/>
     </row>
     <row r="185" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F185" s="46"/>
+      <c r="F185" s="39"/>
       <c r="Q185" s="38"/>
       <c r="R185" s="38"/>
     </row>
     <row r="186" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F186" s="46"/>
+      <c r="F186" s="39"/>
       <c r="Q186" s="38"/>
       <c r="R186" s="38"/>
     </row>
     <row r="187" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F187" s="46"/>
+      <c r="F187" s="39"/>
       <c r="Q187" s="38"/>
       <c r="R187" s="38"/>
     </row>
     <row r="188" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F188" s="46"/>
+      <c r="F188" s="39"/>
       <c r="Q188" s="38"/>
       <c r="R188" s="38"/>
     </row>
     <row r="189" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F189" s="46"/>
+      <c r="F189" s="39"/>
       <c r="Q189" s="38"/>
       <c r="R189" s="38"/>
     </row>
     <row r="190" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F190" s="46"/>
+      <c r="F190" s="39"/>
       <c r="Q190" s="38"/>
       <c r="R190" s="38"/>
     </row>
     <row r="191" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F191" s="46"/>
+      <c r="F191" s="39"/>
       <c r="Q191" s="38"/>
       <c r="R191" s="38"/>
     </row>
     <row r="192" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F192" s="46"/>
+      <c r="F192" s="39"/>
       <c r="Q192" s="38"/>
       <c r="R192" s="38"/>
     </row>
     <row r="193" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F193" s="46"/>
+      <c r="F193" s="39"/>
       <c r="Q193" s="38"/>
       <c r="R193" s="38"/>
     </row>
     <row r="194" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F194" s="46"/>
+      <c r="F194" s="39"/>
       <c r="Q194" s="38"/>
       <c r="R194" s="38"/>
     </row>
     <row r="195" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F195" s="46"/>
+      <c r="F195" s="39"/>
       <c r="Q195" s="38"/>
       <c r="R195" s="38"/>
     </row>
     <row r="196" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F196" s="46"/>
+      <c r="F196" s="39"/>
       <c r="Q196" s="38"/>
       <c r="R196" s="38"/>
     </row>
     <row r="197" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F197" s="46"/>
+      <c r="F197" s="39"/>
       <c r="Q197" s="38"/>
       <c r="R197" s="38"/>
     </row>
     <row r="198" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F198" s="46"/>
+      <c r="F198" s="39"/>
       <c r="Q198" s="38"/>
       <c r="R198" s="38"/>
     </row>
     <row r="199" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F199" s="46"/>
+      <c r="F199" s="39"/>
       <c r="Q199" s="38"/>
       <c r="R199" s="38"/>
     </row>
     <row r="200" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F200" s="46"/>
+      <c r="F200" s="39"/>
       <c r="Q200" s="38"/>
       <c r="R200" s="38"/>
     </row>
     <row r="201" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F201" s="46"/>
+      <c r="F201" s="39"/>
       <c r="Q201" s="38"/>
       <c r="R201" s="38"/>
     </row>
     <row r="202" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F202" s="46"/>
+      <c r="F202" s="39"/>
       <c r="Q202" s="38"/>
       <c r="R202" s="38"/>
     </row>
     <row r="203" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F203" s="46"/>
+      <c r="F203" s="39"/>
       <c r="Q203" s="38"/>
       <c r="R203" s="38"/>
     </row>
     <row r="204" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F204" s="46"/>
+      <c r="F204" s="39"/>
       <c r="Q204" s="38"/>
       <c r="R204" s="38"/>
     </row>
     <row r="205" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F205" s="46"/>
+      <c r="F205" s="39"/>
       <c r="Q205" s="38"/>
       <c r="R205" s="38"/>
     </row>
     <row r="206" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F206" s="46"/>
+      <c r="F206" s="39"/>
       <c r="Q206" s="38"/>
       <c r="R206" s="38"/>
     </row>
     <row r="207" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F207" s="46"/>
+      <c r="F207" s="39"/>
       <c r="Q207" s="38"/>
       <c r="R207" s="38"/>
     </row>
     <row r="208" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F208" s="46"/>
+      <c r="F208" s="39"/>
       <c r="Q208" s="38"/>
       <c r="R208" s="38"/>
     </row>
     <row r="209" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F209" s="46"/>
+      <c r="F209" s="39"/>
       <c r="Q209" s="38"/>
       <c r="R209" s="38"/>
     </row>
     <row r="210" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F210" s="46"/>
+      <c r="F210" s="39"/>
       <c r="Q210" s="38"/>
       <c r="R210" s="38"/>
     </row>
     <row r="211" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F211" s="46"/>
+      <c r="F211" s="39"/>
       <c r="Q211" s="38"/>
       <c r="R211" s="38"/>
     </row>
     <row r="212" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F212" s="46"/>
+      <c r="F212" s="39"/>
       <c r="Q212" s="38"/>
       <c r="R212" s="38"/>
     </row>
     <row r="213" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F213" s="46"/>
+      <c r="F213" s="39"/>
       <c r="Q213" s="38"/>
       <c r="R213" s="38"/>
     </row>
     <row r="214" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F214" s="46"/>
+      <c r="F214" s="39"/>
       <c r="Q214" s="38"/>
       <c r="R214" s="38"/>
     </row>
     <row r="215" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F215" s="46"/>
+      <c r="F215" s="39"/>
       <c r="Q215" s="38"/>
       <c r="R215" s="38"/>
     </row>
     <row r="216" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F216" s="46"/>
+      <c r="F216" s="39"/>
       <c r="Q216" s="38"/>
       <c r="R216" s="38"/>
     </row>
     <row r="217" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F217" s="46"/>
+      <c r="F217" s="39"/>
       <c r="Q217" s="38"/>
       <c r="R217" s="38"/>
     </row>
     <row r="218" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F218" s="46"/>
+      <c r="F218" s="39"/>
       <c r="Q218" s="38"/>
       <c r="R218" s="38"/>
     </row>
     <row r="219" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F219" s="46"/>
+      <c r="F219" s="39"/>
       <c r="Q219" s="38"/>
       <c r="R219" s="38"/>
     </row>
     <row r="220" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F220" s="46"/>
+      <c r="F220" s="39"/>
       <c r="Q220" s="38"/>
       <c r="R220" s="38"/>
     </row>
     <row r="221" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F221" s="46"/>
+      <c r="F221" s="39"/>
       <c r="Q221" s="38"/>
       <c r="R221" s="38"/>
     </row>
     <row r="222" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F222" s="46"/>
+      <c r="F222" s="39"/>
       <c r="Q222" s="38"/>
       <c r="R222" s="38"/>
     </row>
     <row r="223" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F223" s="46"/>
+      <c r="F223" s="39"/>
       <c r="Q223" s="38"/>
       <c r="R223" s="38"/>
     </row>
     <row r="224" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F224" s="46"/>
+      <c r="F224" s="39"/>
       <c r="Q224" s="38"/>
       <c r="R224" s="38"/>
     </row>
     <row r="225" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F225" s="46"/>
+      <c r="F225" s="39"/>
       <c r="Q225" s="38"/>
       <c r="R225" s="38"/>
     </row>
     <row r="226" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F226" s="46"/>
+      <c r="F226" s="39"/>
       <c r="Q226" s="38"/>
       <c r="R226" s="38"/>
     </row>
     <row r="227" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F227" s="46"/>
+      <c r="F227" s="39"/>
       <c r="Q227" s="38"/>
       <c r="R227" s="38"/>
     </row>
     <row r="228" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F228" s="46"/>
+      <c r="F228" s="39"/>
       <c r="Q228" s="38"/>
       <c r="R228" s="38"/>
     </row>
     <row r="229" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F229" s="46"/>
+      <c r="F229" s="39"/>
       <c r="Q229" s="38"/>
       <c r="R229" s="38"/>
     </row>
     <row r="230" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F230" s="46"/>
+      <c r="F230" s="39"/>
       <c r="Q230" s="38"/>
       <c r="R230" s="38"/>
     </row>
     <row r="231" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F231" s="46"/>
+      <c r="F231" s="39"/>
       <c r="Q231" s="38"/>
       <c r="R231" s="38"/>
     </row>
     <row r="232" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F232" s="46"/>
+      <c r="F232" s="39"/>
       <c r="Q232" s="38"/>
       <c r="R232" s="38"/>
     </row>
     <row r="233" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F233" s="46"/>
+      <c r="F233" s="39"/>
       <c r="Q233" s="38"/>
       <c r="R233" s="38"/>
     </row>
     <row r="234" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F234" s="46"/>
+      <c r="F234" s="39"/>
       <c r="Q234" s="38"/>
       <c r="R234" s="38"/>
     </row>
     <row r="235" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F235" s="46"/>
+      <c r="F235" s="39"/>
       <c r="Q235" s="38"/>
       <c r="R235" s="38"/>
     </row>
     <row r="236" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F236" s="46"/>
+      <c r="F236" s="39"/>
       <c r="Q236" s="38"/>
       <c r="R236" s="38"/>
     </row>
     <row r="237" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F237" s="46"/>
+      <c r="F237" s="39"/>
       <c r="Q237" s="38"/>
       <c r="R237" s="38"/>
     </row>
     <row r="238" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F238" s="46"/>
+      <c r="F238" s="39"/>
       <c r="Q238" s="38"/>
       <c r="R238" s="38"/>
     </row>
     <row r="239" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F239" s="46"/>
+      <c r="F239" s="39"/>
       <c r="Q239" s="38"/>
       <c r="R239" s="38"/>
     </row>
     <row r="240" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F240" s="46"/>
+      <c r="F240" s="39"/>
       <c r="Q240" s="38"/>
       <c r="R240" s="38"/>
     </row>
     <row r="241" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F241" s="46"/>
+      <c r="F241" s="39"/>
       <c r="Q241" s="38"/>
       <c r="R241" s="38"/>
     </row>
     <row r="242" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F242" s="46"/>
+      <c r="F242" s="39"/>
       <c r="Q242" s="38"/>
       <c r="R242" s="38"/>
     </row>
     <row r="243" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F243" s="46"/>
+      <c r="F243" s="39"/>
       <c r="Q243" s="38"/>
       <c r="R243" s="38"/>
     </row>
     <row r="244" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F244" s="46"/>
+      <c r="F244" s="39"/>
       <c r="Q244" s="38"/>
       <c r="R244" s="38"/>
     </row>
     <row r="245" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F245" s="46"/>
+      <c r="F245" s="39"/>
       <c r="Q245" s="38"/>
       <c r="R245" s="38"/>
     </row>
     <row r="246" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F246" s="46"/>
+      <c r="F246" s="39"/>
       <c r="Q246" s="38"/>
       <c r="R246" s="38"/>
     </row>
     <row r="247" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F247" s="46"/>
+      <c r="F247" s="39"/>
       <c r="Q247" s="38"/>
       <c r="R247" s="38"/>
     </row>
     <row r="248" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F248" s="46"/>
+      <c r="F248" s="39"/>
       <c r="Q248" s="38"/>
       <c r="R248" s="38"/>
     </row>
     <row r="249" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F249" s="46"/>
+      <c r="F249" s="39"/>
       <c r="Q249" s="38"/>
       <c r="R249" s="38"/>
     </row>
     <row r="250" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F250" s="46"/>
+      <c r="F250" s="39"/>
       <c r="Q250" s="38"/>
       <c r="R250" s="38"/>
     </row>
     <row r="251" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F251" s="46"/>
+      <c r="F251" s="39"/>
       <c r="Q251" s="38"/>
       <c r="R251" s="38"/>
     </row>
     <row r="252" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F252" s="46"/>
+      <c r="F252" s="39"/>
       <c r="Q252" s="38"/>
       <c r="R252" s="38"/>
     </row>
     <row r="253" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F253" s="46"/>
+      <c r="F253" s="39"/>
       <c r="Q253" s="38"/>
       <c r="R253" s="38"/>
     </row>
     <row r="254" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F254" s="46"/>
+      <c r="F254" s="39"/>
       <c r="Q254" s="38"/>
       <c r="R254" s="38"/>
     </row>
     <row r="255" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F255" s="46"/>
+      <c r="F255" s="39"/>
       <c r="Q255" s="38"/>
       <c r="R255" s="38"/>
     </row>
     <row r="256" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F256" s="46"/>
+      <c r="F256" s="39"/>
       <c r="Q256" s="38"/>
       <c r="R256" s="38"/>
     </row>
     <row r="257" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F257" s="46"/>
+      <c r="F257" s="39"/>
       <c r="Q257" s="38"/>
       <c r="R257" s="38"/>
     </row>
     <row r="258" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F258" s="46"/>
+      <c r="F258" s="39"/>
       <c r="Q258" s="38"/>
       <c r="R258" s="38"/>
     </row>
     <row r="259" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F259" s="46"/>
+      <c r="F259" s="39"/>
       <c r="Q259" s="38"/>
       <c r="R259" s="38"/>
     </row>
     <row r="260" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F260" s="46"/>
+      <c r="F260" s="39"/>
       <c r="Q260" s="38"/>
       <c r="R260" s="38"/>
     </row>
     <row r="261" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F261" s="46"/>
+      <c r="F261" s="39"/>
       <c r="Q261" s="38"/>
       <c r="R261" s="38"/>
     </row>
     <row r="262" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F262" s="46"/>
+      <c r="F262" s="39"/>
       <c r="Q262" s="38"/>
       <c r="R262" s="38"/>
     </row>
     <row r="263" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F263" s="46"/>
+      <c r="F263" s="39"/>
       <c r="Q263" s="38"/>
       <c r="R263" s="38"/>
     </row>
     <row r="264" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F264" s="46"/>
+      <c r="F264" s="39"/>
       <c r="Q264" s="38"/>
       <c r="R264" s="38"/>
     </row>
     <row r="265" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F265" s="46"/>
+      <c r="F265" s="39"/>
       <c r="Q265" s="38"/>
       <c r="R265" s="38"/>
     </row>
     <row r="266" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F266" s="46"/>
+      <c r="F266" s="39"/>
       <c r="Q266" s="38"/>
       <c r="R266" s="38"/>
     </row>
     <row r="267" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F267" s="46"/>
+      <c r="F267" s="39"/>
       <c r="Q267" s="38"/>
       <c r="R267" s="38"/>
     </row>
     <row r="268" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F268" s="46"/>
+      <c r="F268" s="39"/>
       <c r="Q268" s="38"/>
       <c r="R268" s="38"/>
     </row>
     <row r="269" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F269" s="46"/>
+      <c r="F269" s="39"/>
       <c r="Q269" s="38"/>
       <c r="R269" s="38"/>
     </row>
     <row r="270" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F270" s="46"/>
+      <c r="F270" s="39"/>
       <c r="Q270" s="38"/>
       <c r="R270" s="38"/>
     </row>
     <row r="271" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F271" s="46"/>
+      <c r="F271" s="39"/>
       <c r="Q271" s="38"/>
       <c r="R271" s="38"/>
     </row>
     <row r="272" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F272" s="46"/>
+      <c r="F272" s="39"/>
       <c r="Q272" s="38"/>
       <c r="R272" s="38"/>
     </row>
     <row r="273" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F273" s="46"/>
+      <c r="F273" s="39"/>
       <c r="Q273" s="38"/>
       <c r="R273" s="38"/>
     </row>
     <row r="274" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F274" s="46"/>
+      <c r="F274" s="39"/>
       <c r="Q274" s="38"/>
       <c r="R274" s="38"/>
     </row>
     <row r="275" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F275" s="46"/>
+      <c r="F275" s="39"/>
       <c r="Q275" s="38"/>
       <c r="R275" s="38"/>
     </row>
     <row r="276" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F276" s="46"/>
+      <c r="F276" s="39"/>
       <c r="Q276" s="38"/>
       <c r="R276" s="38"/>
     </row>
     <row r="277" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F277" s="46"/>
+      <c r="F277" s="39"/>
       <c r="Q277" s="38"/>
       <c r="R277" s="38"/>
     </row>
     <row r="278" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F278" s="46"/>
+      <c r="F278" s="39"/>
       <c r="Q278" s="38"/>
       <c r="R278" s="38"/>
     </row>
     <row r="279" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F279" s="46"/>
+      <c r="F279" s="39"/>
       <c r="Q279" s="38"/>
       <c r="R279" s="38"/>
     </row>
     <row r="280" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F280" s="46"/>
+      <c r="F280" s="39"/>
       <c r="Q280" s="38"/>
       <c r="R280" s="38"/>
     </row>
     <row r="281" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F281" s="46"/>
+      <c r="F281" s="39"/>
       <c r="Q281" s="38"/>
       <c r="R281" s="38"/>
     </row>
     <row r="282" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F282" s="46"/>
+      <c r="F282" s="39"/>
       <c r="Q282" s="38"/>
       <c r="R282" s="38"/>
     </row>
     <row r="283" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F283" s="46"/>
+      <c r="F283" s="39"/>
       <c r="Q283" s="38"/>
       <c r="R283" s="38"/>
     </row>
     <row r="284" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F284" s="46"/>
+      <c r="F284" s="39"/>
       <c r="Q284" s="38"/>
       <c r="R284" s="38"/>
     </row>
     <row r="285" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F285" s="46"/>
+      <c r="F285" s="39"/>
       <c r="Q285" s="38"/>
       <c r="R285" s="38"/>
     </row>
     <row r="286" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F286" s="46"/>
+      <c r="F286" s="39"/>
       <c r="Q286" s="38"/>
       <c r="R286" s="38"/>
     </row>
     <row r="287" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F287" s="46"/>
+      <c r="F287" s="39"/>
       <c r="Q287" s="38"/>
       <c r="R287" s="38"/>
     </row>
     <row r="288" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F288" s="46"/>
+      <c r="F288" s="39"/>
       <c r="Q288" s="38"/>
       <c r="R288" s="38"/>
     </row>
     <row r="289" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F289" s="46"/>
+      <c r="F289" s="39"/>
       <c r="Q289" s="38"/>
       <c r="R289" s="38"/>
     </row>
     <row r="290" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F290" s="46"/>
+      <c r="F290" s="39"/>
       <c r="Q290" s="38"/>
       <c r="R290" s="38"/>
     </row>
     <row r="291" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F291" s="46"/>
+      <c r="F291" s="39"/>
       <c r="Q291" s="38"/>
       <c r="R291" s="38"/>
     </row>
     <row r="292" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F292" s="46"/>
+      <c r="F292" s="39"/>
       <c r="Q292" s="38"/>
       <c r="R292" s="38"/>
     </row>
     <row r="293" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F293" s="46"/>
+      <c r="F293" s="39"/>
       <c r="Q293" s="38"/>
       <c r="R293" s="38"/>
     </row>
     <row r="294" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F294" s="46"/>
+      <c r="F294" s="39"/>
       <c r="Q294" s="38"/>
       <c r="R294" s="38"/>
     </row>
     <row r="295" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F295" s="46"/>
+      <c r="F295" s="39"/>
       <c r="Q295" s="38"/>
       <c r="R295" s="38"/>
     </row>
     <row r="296" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F296" s="46"/>
+      <c r="F296" s="39"/>
       <c r="Q296" s="38"/>
       <c r="R296" s="38"/>
     </row>
     <row r="297" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F297" s="46"/>
+      <c r="F297" s="39"/>
       <c r="Q297" s="38"/>
       <c r="R297" s="38"/>
     </row>
     <row r="298" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F298" s="46"/>
+      <c r="F298" s="39"/>
       <c r="Q298" s="38"/>
       <c r="R298" s="38"/>
     </row>
     <row r="299" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F299" s="46"/>
+      <c r="F299" s="39"/>
       <c r="Q299" s="38"/>
       <c r="R299" s="38"/>
     </row>
     <row r="300" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F300" s="46"/>
+      <c r="F300" s="39"/>
       <c r="Q300" s="38"/>
       <c r="R300" s="38"/>
     </row>
     <row r="301" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F301" s="46"/>
+      <c r="F301" s="39"/>
       <c r="Q301" s="38"/>
       <c r="R301" s="38"/>
     </row>
     <row r="302" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F302" s="46"/>
+      <c r="F302" s="39"/>
       <c r="Q302" s="38"/>
       <c r="R302" s="38"/>
     </row>
     <row r="303" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F303" s="46"/>
+      <c r="F303" s="39"/>
       <c r="Q303" s="38"/>
       <c r="R303" s="38"/>
     </row>
     <row r="304" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F304" s="46"/>
+      <c r="F304" s="39"/>
       <c r="Q304" s="38"/>
       <c r="R304" s="38"/>
     </row>
     <row r="305" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F305" s="46"/>
+      <c r="F305" s="39"/>
       <c r="Q305" s="38"/>
       <c r="R305" s="38"/>
     </row>
     <row r="306" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F306" s="46"/>
+      <c r="F306" s="39"/>
       <c r="Q306" s="38"/>
       <c r="R306" s="38"/>
     </row>
     <row r="307" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F307" s="46"/>
+      <c r="F307" s="39"/>
       <c r="Q307" s="38"/>
       <c r="R307" s="38"/>
     </row>
     <row r="308" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F308" s="46"/>
+      <c r="F308" s="39"/>
       <c r="Q308" s="38"/>
       <c r="R308" s="38"/>
     </row>
     <row r="309" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F309" s="46"/>
+      <c r="F309" s="39"/>
       <c r="Q309" s="38"/>
       <c r="R309" s="38"/>
     </row>
     <row r="310" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F310" s="46"/>
+      <c r="F310" s="39"/>
       <c r="Q310" s="38"/>
       <c r="R310" s="38"/>
     </row>
     <row r="311" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F311" s="46"/>
+      <c r="F311" s="39"/>
       <c r="Q311" s="38"/>
       <c r="R311" s="38"/>
     </row>
     <row r="312" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F312" s="46"/>
+      <c r="F312" s="39"/>
       <c r="Q312" s="38"/>
       <c r="R312" s="38"/>
     </row>
     <row r="313" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F313" s="46"/>
+      <c r="F313" s="39"/>
       <c r="Q313" s="38"/>
       <c r="R313" s="38"/>
     </row>
     <row r="314" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F314" s="46"/>
+      <c r="F314" s="39"/>
       <c r="Q314" s="38"/>
       <c r="R314" s="38"/>
     </row>
     <row r="315" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F315" s="46"/>
+      <c r="F315" s="39"/>
       <c r="Q315" s="38"/>
       <c r="R315" s="38"/>
     </row>
     <row r="316" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F316" s="46"/>
+      <c r="F316" s="39"/>
       <c r="Q316" s="38"/>
       <c r="R316" s="38"/>
     </row>
     <row r="317" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F317" s="46"/>
+      <c r="F317" s="39"/>
       <c r="Q317" s="38"/>
       <c r="R317" s="38"/>
     </row>
     <row r="318" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F318" s="46"/>
+      <c r="F318" s="39"/>
       <c r="Q318" s="38"/>
       <c r="R318" s="38"/>
     </row>
     <row r="319" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F319" s="46"/>
+      <c r="F319" s="39"/>
       <c r="Q319" s="38"/>
       <c r="R319" s="38"/>
     </row>
     <row r="320" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F320" s="46"/>
+      <c r="F320" s="39"/>
       <c r="Q320" s="38"/>
       <c r="R320" s="38"/>
     </row>
     <row r="321" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F321" s="46"/>
+      <c r="F321" s="39"/>
       <c r="Q321" s="38"/>
       <c r="R321" s="38"/>
     </row>
     <row r="322" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F322" s="46"/>
+      <c r="F322" s="39"/>
       <c r="Q322" s="38"/>
       <c r="R322" s="38"/>
     </row>
     <row r="323" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F323" s="46"/>
+      <c r="F323" s="39"/>
       <c r="Q323" s="38"/>
       <c r="R323" s="38"/>
     </row>
     <row r="324" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F324" s="46"/>
+      <c r="F324" s="39"/>
       <c r="Q324" s="38"/>
       <c r="R324" s="38"/>
     </row>
     <row r="325" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F325" s="46"/>
+      <c r="F325" s="39"/>
       <c r="Q325" s="38"/>
       <c r="R325" s="38"/>
     </row>
     <row r="326" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F326" s="46"/>
+      <c r="F326" s="39"/>
       <c r="Q326" s="38"/>
       <c r="R326" s="38"/>
     </row>
     <row r="327" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F327" s="46"/>
+      <c r="F327" s="39"/>
       <c r="Q327" s="38"/>
       <c r="R327" s="38"/>
     </row>
     <row r="328" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F328" s="46"/>
+      <c r="F328" s="39"/>
       <c r="Q328" s="38"/>
       <c r="R328" s="38"/>
     </row>
     <row r="329" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F329" s="46"/>
+      <c r="F329" s="39"/>
       <c r="Q329" s="38"/>
       <c r="R329" s="38"/>
     </row>
     <row r="330" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F330" s="46"/>
+      <c r="F330" s="39"/>
       <c r="Q330" s="38"/>
       <c r="R330" s="38"/>
     </row>
     <row r="331" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F331" s="46"/>
+      <c r="F331" s="39"/>
       <c r="Q331" s="38"/>
       <c r="R331" s="38"/>
     </row>
     <row r="332" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F332" s="46"/>
+      <c r="F332" s="39"/>
       <c r="Q332" s="38"/>
       <c r="R332" s="38"/>
     </row>
     <row r="333" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F333" s="46"/>
+      <c r="F333" s="39"/>
       <c r="Q333" s="38"/>
       <c r="R333" s="38"/>
     </row>
     <row r="334" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F334" s="46"/>
+      <c r="F334" s="39"/>
       <c r="Q334" s="38"/>
       <c r="R334" s="38"/>
     </row>
     <row r="335" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F335" s="46"/>
+      <c r="F335" s="39"/>
       <c r="Q335" s="38"/>
       <c r="R335" s="38"/>
     </row>
     <row r="336" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F336" s="46"/>
+      <c r="F336" s="39"/>
       <c r="Q336" s="38"/>
       <c r="R336" s="38"/>
     </row>
@@ -8474,718 +8477,1620 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P18"/>
+  <dimension ref="B3:P34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="50">
+      <c r="C4" s="43">
         <v>0.03</v>
       </c>
-      <c r="D4" s="50">
+      <c r="D4" s="43">
         <v>3.15E-2</v>
       </c>
-      <c r="E4" s="50">
+      <c r="E4" s="43">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="F4" s="50">
+      <c r="F4" s="43">
         <v>3.4500000000000003E-2</v>
       </c>
-      <c r="G4" s="50">
+      <c r="G4" s="43">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="H4" s="50">
+      <c r="H4" s="43">
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="I4" s="50">
+      <c r="I4" s="43">
         <v>3.9E-2</v>
       </c>
-      <c r="J4" s="50">
+      <c r="J4" s="43">
         <v>4.0500000000000001E-2</v>
       </c>
-      <c r="K4" s="50">
+      <c r="K4" s="43">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="L4" s="50">
+      <c r="L4" s="43">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="M4" s="50">
+      <c r="M4" s="43">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="N4" s="50">
+      <c r="N4" s="43">
         <v>4.65E-2</v>
       </c>
-      <c r="O4" s="50">
+      <c r="O4" s="43">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="P4" s="51">
+      <c r="P4" s="44">
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="53">
+      <c r="C5" s="46">
         <v>468364</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="47">
         <v>470028</v>
       </c>
-      <c r="E5" s="54">
+      <c r="E5" s="47">
         <v>471276</v>
       </c>
-      <c r="F5" s="54">
+      <c r="F5" s="47">
         <v>472160</v>
       </c>
-      <c r="G5" s="54">
+      <c r="G5" s="47">
         <v>472732</v>
       </c>
-      <c r="H5" s="54">
+      <c r="H5" s="47">
         <v>472940</v>
       </c>
-      <c r="I5" s="54">
+      <c r="I5" s="47">
         <v>472940</v>
       </c>
-      <c r="J5" s="54">
+      <c r="J5" s="47">
         <v>472732</v>
       </c>
-      <c r="K5" s="54">
+      <c r="K5" s="47">
         <v>472420</v>
       </c>
-      <c r="L5" s="54">
+      <c r="L5" s="47">
         <v>471952</v>
       </c>
-      <c r="M5" s="54">
+      <c r="M5" s="47">
         <v>471432</v>
       </c>
-      <c r="N5" s="54">
+      <c r="N5" s="47">
         <v>470704</v>
       </c>
-      <c r="O5" s="54">
+      <c r="O5" s="47">
         <v>469924</v>
       </c>
-      <c r="P5" s="55">
+      <c r="P5" s="48">
         <v>469092</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="56">
+      <c r="C6" s="49">
         <v>433056</v>
       </c>
-      <c r="D6" s="57">
+      <c r="D6" s="50">
         <v>434824</v>
       </c>
-      <c r="E6" s="57">
+      <c r="E6" s="50">
         <v>435916</v>
       </c>
-      <c r="F6" s="57">
+      <c r="F6" s="50">
         <v>436436</v>
       </c>
-      <c r="G6" s="57">
+      <c r="G6" s="50">
         <v>436644</v>
       </c>
-      <c r="H6" s="57">
+      <c r="H6" s="50">
         <v>436592</v>
       </c>
-      <c r="I6" s="57">
+      <c r="I6" s="50">
         <v>436332</v>
       </c>
-      <c r="J6" s="57">
+      <c r="J6" s="50">
         <v>435864</v>
       </c>
-      <c r="K6" s="57">
+      <c r="K6" s="50">
         <v>435240</v>
       </c>
-      <c r="L6" s="57">
+      <c r="L6" s="50">
         <v>434408</v>
       </c>
-      <c r="M6" s="57">
+      <c r="M6" s="50">
         <v>433368</v>
       </c>
-      <c r="N6" s="57">
+      <c r="N6" s="50">
         <v>432224</v>
       </c>
-      <c r="O6" s="57">
+      <c r="O6" s="50">
         <v>430924</v>
       </c>
-      <c r="P6" s="58">
+      <c r="P6" s="51">
         <v>429468</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="56">
+      <c r="C7" s="49">
         <v>378560</v>
       </c>
-      <c r="D7" s="57">
+      <c r="D7" s="50">
         <v>379808</v>
       </c>
-      <c r="E7" s="57">
+      <c r="E7" s="50">
         <v>380484</v>
       </c>
-      <c r="F7" s="57">
+      <c r="F7" s="50">
         <v>380796</v>
       </c>
-      <c r="G7" s="57">
+      <c r="G7" s="50">
         <v>380900</v>
       </c>
-      <c r="H7" s="57">
+      <c r="H7" s="50">
         <v>380744</v>
       </c>
-      <c r="I7" s="57">
+      <c r="I7" s="50">
         <v>380432</v>
       </c>
-      <c r="J7" s="57">
+      <c r="J7" s="50">
         <v>379912</v>
       </c>
-      <c r="K7" s="57">
+      <c r="K7" s="50">
         <v>379236</v>
       </c>
-      <c r="L7" s="57">
+      <c r="L7" s="50">
         <v>378352</v>
       </c>
-      <c r="M7" s="57">
+      <c r="M7" s="50">
         <v>377260</v>
       </c>
-      <c r="N7" s="57">
+      <c r="N7" s="50">
         <v>376012</v>
       </c>
-      <c r="O7" s="57">
+      <c r="O7" s="50">
         <v>374660</v>
       </c>
-      <c r="P7" s="58">
+      <c r="P7" s="51">
         <v>373100</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="56">
+      <c r="C8" s="49">
         <v>432068</v>
       </c>
-      <c r="D8" s="57">
+      <c r="D8" s="50">
         <v>433680</v>
       </c>
-      <c r="E8" s="57">
+      <c r="E8" s="50">
         <v>434876</v>
       </c>
-      <c r="F8" s="57">
+      <c r="F8" s="50">
         <v>435656</v>
       </c>
-      <c r="G8" s="57">
+      <c r="G8" s="50">
         <v>436020</v>
       </c>
-      <c r="H8" s="57">
+      <c r="H8" s="50">
         <v>436124</v>
       </c>
-      <c r="I8" s="57">
+      <c r="I8" s="50">
         <v>435968</v>
       </c>
-      <c r="J8" s="57">
+      <c r="J8" s="50">
         <v>435656</v>
       </c>
-      <c r="K8" s="57">
+      <c r="K8" s="50">
         <v>435136</v>
       </c>
-      <c r="L8" s="57">
+      <c r="L8" s="50">
         <v>434408</v>
       </c>
-      <c r="M8" s="57">
+      <c r="M8" s="50">
         <v>433524</v>
       </c>
-      <c r="N8" s="57">
+      <c r="N8" s="50">
         <v>432484</v>
       </c>
-      <c r="O8" s="57">
+      <c r="O8" s="50">
         <v>431340</v>
       </c>
-      <c r="P8" s="58">
+      <c r="P8" s="51">
         <v>430092</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="56">
+      <c r="C9" s="49">
         <v>380900</v>
       </c>
-      <c r="D9" s="57">
+      <c r="D9" s="50">
         <v>382460</v>
       </c>
-      <c r="E9" s="57">
+      <c r="E9" s="50">
         <v>383708</v>
       </c>
-      <c r="F9" s="57">
+      <c r="F9" s="50">
         <v>384592</v>
       </c>
-      <c r="G9" s="57">
+      <c r="G9" s="50">
         <v>385060</v>
       </c>
-      <c r="H9" s="57">
+      <c r="H9" s="50">
         <v>385216</v>
       </c>
-      <c r="I9" s="57">
+      <c r="I9" s="50">
         <v>385164</v>
       </c>
-      <c r="J9" s="57">
+      <c r="J9" s="50">
         <v>385008</v>
       </c>
-      <c r="K9" s="57">
+      <c r="K9" s="50">
         <v>384644</v>
       </c>
-      <c r="L9" s="57">
+      <c r="L9" s="50">
         <v>384176</v>
       </c>
-      <c r="M9" s="57">
+      <c r="M9" s="50">
         <v>383604</v>
       </c>
-      <c r="N9" s="57">
+      <c r="N9" s="50">
         <v>382876</v>
       </c>
-      <c r="O9" s="57">
+      <c r="O9" s="50">
         <v>382044</v>
       </c>
-      <c r="P9" s="58">
+      <c r="P9" s="51">
         <v>381160</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="56">
+      <c r="C10" s="49">
         <v>459264</v>
       </c>
-      <c r="D10" s="57">
+      <c r="D10" s="50">
         <v>460824</v>
       </c>
-      <c r="E10" s="57">
+      <c r="E10" s="50">
         <v>461968</v>
       </c>
-      <c r="F10" s="57">
+      <c r="F10" s="50">
         <v>462800</v>
       </c>
-      <c r="G10" s="57">
+      <c r="G10" s="50">
         <v>463268</v>
       </c>
-      <c r="H10" s="57">
+      <c r="H10" s="50">
         <v>463424</v>
       </c>
-      <c r="I10" s="57">
+      <c r="I10" s="50">
         <v>463424</v>
       </c>
-      <c r="J10" s="57">
+      <c r="J10" s="50">
         <v>463216</v>
       </c>
-      <c r="K10" s="57">
+      <c r="K10" s="50">
         <v>462800</v>
       </c>
-      <c r="L10" s="57">
+      <c r="L10" s="50">
         <v>462228</v>
       </c>
-      <c r="M10" s="57">
+      <c r="M10" s="50">
         <v>461500</v>
       </c>
-      <c r="N10" s="57">
+      <c r="N10" s="50">
         <v>460616</v>
       </c>
-      <c r="O10" s="57">
+      <c r="O10" s="50">
         <v>459628</v>
       </c>
-      <c r="P10" s="58">
+      <c r="P10" s="51">
         <v>458536</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="56">
+      <c r="C11" s="49">
         <v>463892</v>
       </c>
-      <c r="D11" s="57">
+      <c r="D11" s="50">
         <v>465244</v>
       </c>
-      <c r="E11" s="57">
+      <c r="E11" s="50">
         <v>466284</v>
       </c>
-      <c r="F11" s="57">
+      <c r="F11" s="50">
         <v>466960</v>
       </c>
-      <c r="G11" s="57">
+      <c r="G11" s="50">
         <v>467376</v>
       </c>
-      <c r="H11" s="57">
+      <c r="H11" s="50">
         <v>467532</v>
       </c>
-      <c r="I11" s="57">
+      <c r="I11" s="50">
         <v>467480</v>
       </c>
-      <c r="J11" s="57">
+      <c r="J11" s="50">
         <v>467168</v>
       </c>
-      <c r="K11" s="57">
+      <c r="K11" s="50">
         <v>466648</v>
       </c>
-      <c r="L11" s="57">
+      <c r="L11" s="50">
         <v>466024</v>
       </c>
-      <c r="M11" s="57">
+      <c r="M11" s="50">
         <v>465140</v>
       </c>
-      <c r="N11" s="57">
+      <c r="N11" s="50">
         <v>464152</v>
       </c>
-      <c r="O11" s="57">
+      <c r="O11" s="50">
         <v>462956</v>
       </c>
-      <c r="P11" s="58">
+      <c r="P11" s="51">
         <v>461656</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="56">
+      <c r="C12" s="49">
         <v>404664</v>
       </c>
-      <c r="D12" s="57">
+      <c r="D12" s="50">
         <v>406224</v>
       </c>
-      <c r="E12" s="57">
+      <c r="E12" s="50">
         <v>407420</v>
       </c>
-      <c r="F12" s="57">
+      <c r="F12" s="50">
         <v>408200</v>
       </c>
-      <c r="G12" s="57">
+      <c r="G12" s="50">
         <v>408616</v>
       </c>
-      <c r="H12" s="57">
+      <c r="H12" s="50">
         <v>408772</v>
       </c>
-      <c r="I12" s="57">
+      <c r="I12" s="50">
         <v>408720</v>
       </c>
-      <c r="J12" s="57">
+      <c r="J12" s="50">
         <v>408512</v>
       </c>
-      <c r="K12" s="57">
+      <c r="K12" s="50">
         <v>408148</v>
       </c>
-      <c r="L12" s="57">
+      <c r="L12" s="50">
         <v>407628</v>
       </c>
-      <c r="M12" s="57">
+      <c r="M12" s="50">
         <v>407004</v>
       </c>
-      <c r="N12" s="57">
+      <c r="N12" s="50">
         <v>406276</v>
       </c>
-      <c r="O12" s="57">
+      <c r="O12" s="50">
         <v>405444</v>
       </c>
-      <c r="P12" s="58">
+      <c r="P12" s="51">
         <v>404508</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="56">
+      <c r="C13" s="49">
         <v>441220</v>
       </c>
-      <c r="D13" s="57">
+      <c r="D13" s="50">
         <v>443300</v>
       </c>
-      <c r="E13" s="57">
+      <c r="E13" s="50">
         <v>444912</v>
       </c>
-      <c r="F13" s="57">
+      <c r="F13" s="50">
         <v>446056</v>
       </c>
-      <c r="G13" s="57">
+      <c r="G13" s="50">
         <v>446888</v>
       </c>
-      <c r="H13" s="57">
+      <c r="H13" s="50">
         <v>447356</v>
       </c>
-      <c r="I13" s="57">
+      <c r="I13" s="50">
         <v>447564</v>
       </c>
-      <c r="J13" s="57">
+      <c r="J13" s="50">
         <v>447512</v>
       </c>
-      <c r="K13" s="57">
+      <c r="K13" s="50">
         <v>447200</v>
       </c>
-      <c r="L13" s="57">
+      <c r="L13" s="50">
         <v>446732</v>
       </c>
-      <c r="M13" s="57">
+      <c r="M13" s="50">
         <v>445900</v>
       </c>
-      <c r="N13" s="57">
+      <c r="N13" s="50">
         <v>444912</v>
       </c>
-      <c r="O13" s="57">
+      <c r="O13" s="50">
         <v>443612</v>
       </c>
-      <c r="P13" s="58">
+      <c r="P13" s="51">
         <v>442104</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="56">
+      <c r="C14" s="49">
         <v>450528</v>
       </c>
-      <c r="D14" s="57">
+      <c r="D14" s="50">
         <v>452608</v>
       </c>
-      <c r="E14" s="57">
+      <c r="E14" s="50">
         <v>453596</v>
       </c>
-      <c r="F14" s="57">
+      <c r="F14" s="50">
         <v>453908</v>
       </c>
-      <c r="G14" s="57">
+      <c r="G14" s="50">
         <v>454012</v>
       </c>
-      <c r="H14" s="57">
+      <c r="H14" s="50">
         <v>453856</v>
       </c>
-      <c r="I14" s="57">
+      <c r="I14" s="50">
         <v>453544</v>
       </c>
-      <c r="J14" s="57">
+      <c r="J14" s="50">
         <v>452972</v>
       </c>
-      <c r="K14" s="57">
+      <c r="K14" s="50">
         <v>452192</v>
       </c>
-      <c r="L14" s="57">
+      <c r="L14" s="50">
         <v>451256</v>
       </c>
-      <c r="M14" s="57">
+      <c r="M14" s="50">
         <v>450164</v>
       </c>
-      <c r="N14" s="57">
+      <c r="N14" s="50">
         <v>448916</v>
       </c>
-      <c r="O14" s="57">
+      <c r="O14" s="50">
         <v>447460</v>
       </c>
-      <c r="P14" s="58">
+      <c r="P14" s="51">
         <v>445848</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="56">
+      <c r="C15" s="49">
         <v>468000</v>
       </c>
-      <c r="D15" s="57">
+      <c r="D15" s="50">
         <v>469612</v>
       </c>
-      <c r="E15" s="57">
+      <c r="E15" s="50">
         <v>470860</v>
       </c>
-      <c r="F15" s="57">
+      <c r="F15" s="50">
         <v>471744</v>
       </c>
-      <c r="G15" s="57">
+      <c r="G15" s="50">
         <v>472316</v>
       </c>
-      <c r="H15" s="57">
+      <c r="H15" s="50">
         <v>472524</v>
       </c>
-      <c r="I15" s="57">
+      <c r="I15" s="50">
         <v>472472</v>
       </c>
-      <c r="J15" s="57">
+      <c r="J15" s="50">
         <v>472264</v>
       </c>
-      <c r="K15" s="57">
+      <c r="K15" s="50">
         <v>471900</v>
       </c>
-      <c r="L15" s="57">
+      <c r="L15" s="50">
         <v>471380</v>
       </c>
-      <c r="M15" s="57">
+      <c r="M15" s="50">
         <v>470756</v>
       </c>
-      <c r="N15" s="57">
+      <c r="N15" s="50">
         <v>470028</v>
       </c>
-      <c r="O15" s="57">
+      <c r="O15" s="50">
         <v>469144</v>
       </c>
-      <c r="P15" s="58">
+      <c r="P15" s="51">
         <v>468208</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="56">
+      <c r="C16" s="49">
         <v>436956</v>
       </c>
-      <c r="D16" s="57">
+      <c r="D16" s="50">
         <v>439660</v>
       </c>
-      <c r="E16" s="57">
+      <c r="E16" s="50">
         <v>442000</v>
       </c>
-      <c r="F16" s="57">
+      <c r="F16" s="50">
         <v>444028</v>
       </c>
-      <c r="G16" s="57">
+      <c r="G16" s="50">
         <v>445692</v>
       </c>
-      <c r="H16" s="57">
+      <c r="H16" s="50">
         <v>447044</v>
       </c>
-      <c r="I16" s="57">
+      <c r="I16" s="50">
         <v>448084</v>
       </c>
-      <c r="J16" s="57">
+      <c r="J16" s="50">
         <v>448916</v>
       </c>
-      <c r="K16" s="57">
+      <c r="K16" s="50">
         <v>449436</v>
       </c>
-      <c r="L16" s="57">
+      <c r="L16" s="50">
         <v>449748</v>
       </c>
-      <c r="M16" s="57">
+      <c r="M16" s="50">
         <v>449904</v>
       </c>
-      <c r="N16" s="57">
+      <c r="N16" s="50">
         <v>449956</v>
       </c>
-      <c r="O16" s="57">
+      <c r="O16" s="50">
         <v>449904</v>
       </c>
-      <c r="P16" s="58">
+      <c r="P16" s="51">
         <v>449748</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="56">
+      <c r="C17" s="49">
         <v>506005.76000000001</v>
       </c>
-      <c r="D17" s="57">
+      <c r="D17" s="50">
         <v>509254.39999999997</v>
       </c>
-      <c r="E17" s="57">
+      <c r="E17" s="50">
         <v>512021.76000000001</v>
       </c>
-      <c r="F17" s="57">
+      <c r="F17" s="50">
         <v>514428.16000000003</v>
       </c>
-      <c r="G17" s="57">
+      <c r="G17" s="50">
         <v>516473.59999999998</v>
       </c>
-      <c r="H17" s="57">
+      <c r="H17" s="50">
         <v>518097.91999999998</v>
       </c>
-      <c r="I17" s="57">
+      <c r="I17" s="50">
         <v>519421.44</v>
       </c>
-      <c r="J17" s="57">
+      <c r="J17" s="50">
         <v>520444.16000000003</v>
       </c>
-      <c r="K17" s="57">
+      <c r="K17" s="50">
         <v>521105.91999999998</v>
       </c>
-      <c r="L17" s="57">
+      <c r="L17" s="50">
         <v>521647.36000000004</v>
       </c>
-      <c r="M17" s="57">
+      <c r="M17" s="50">
         <v>522008.32000000001</v>
       </c>
-      <c r="N17" s="57">
+      <c r="N17" s="50">
         <v>522309.12</v>
       </c>
-      <c r="O17" s="57">
+      <c r="O17" s="50">
         <v>522489.60000000009</v>
       </c>
-      <c r="P17" s="58">
+      <c r="P17" s="51">
         <v>522549.76000000007</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="60">
+      <c r="C18" s="53">
         <v>448974.07999999996</v>
       </c>
-      <c r="D18" s="61">
+      <c r="D18" s="54">
         <v>451380.47999999998</v>
       </c>
-      <c r="E18" s="61">
+      <c r="E18" s="54">
         <v>453245.43999999994</v>
       </c>
-      <c r="F18" s="61">
+      <c r="F18" s="54">
         <v>454508.79999999999</v>
       </c>
-      <c r="G18" s="61">
+      <c r="G18" s="54">
         <v>455290.88</v>
       </c>
-      <c r="H18" s="61">
+      <c r="H18" s="54">
         <v>455651.83999999997</v>
       </c>
-      <c r="I18" s="61">
+      <c r="I18" s="54">
         <v>455772.16000000009</v>
       </c>
-      <c r="J18" s="61">
+      <c r="J18" s="54">
         <v>455651.83999999997</v>
       </c>
-      <c r="K18" s="61">
+      <c r="K18" s="54">
         <v>455170.56</v>
       </c>
-      <c r="L18" s="61">
+      <c r="L18" s="54">
         <v>454508.79999999999</v>
       </c>
-      <c r="M18" s="61">
+      <c r="M18" s="54">
         <v>453546.24000000005</v>
       </c>
-      <c r="N18" s="61">
+      <c r="N18" s="54">
         <v>452282.88</v>
       </c>
-      <c r="O18" s="61">
+      <c r="O18" s="54">
         <v>450658.56000000006</v>
       </c>
-      <c r="P18" s="62">
+      <c r="P18" s="55">
         <v>448853.75999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="43">
+        <v>0.03</v>
+      </c>
+      <c r="D20" s="43">
+        <v>3.15E-2</v>
+      </c>
+      <c r="E20" s="43">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F20" s="43">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="G20" s="43">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="H20" s="43">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="I20" s="43">
+        <v>3.9E-2</v>
+      </c>
+      <c r="J20" s="43">
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="K20" s="43">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="L20" s="43">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="M20" s="43">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="N20" s="43">
+        <v>4.65E-2</v>
+      </c>
+      <c r="O20" s="43">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="P20" s="44">
+        <v>4.9500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="46">
+        <f>C5/365.25</f>
+        <v>1282.3107460643396</v>
+      </c>
+      <c r="D21" s="47">
+        <f t="shared" ref="D21:P21" si="0">D5/365.25</f>
+        <v>1286.8665297741272</v>
+      </c>
+      <c r="E21" s="47">
+        <f t="shared" si="0"/>
+        <v>1290.2833675564682</v>
+      </c>
+      <c r="F21" s="47">
+        <f t="shared" si="0"/>
+        <v>1292.7036276522929</v>
+      </c>
+      <c r="G21" s="47">
+        <f t="shared" si="0"/>
+        <v>1294.2696783025326</v>
+      </c>
+      <c r="H21" s="47">
+        <f t="shared" si="0"/>
+        <v>1294.8391512662561</v>
+      </c>
+      <c r="I21" s="47">
+        <f t="shared" si="0"/>
+        <v>1294.8391512662561</v>
+      </c>
+      <c r="J21" s="47">
+        <f t="shared" si="0"/>
+        <v>1294.2696783025326</v>
+      </c>
+      <c r="K21" s="47">
+        <f t="shared" si="0"/>
+        <v>1293.4154688569472</v>
+      </c>
+      <c r="L21" s="47">
+        <f t="shared" si="0"/>
+        <v>1292.1341546885694</v>
+      </c>
+      <c r="M21" s="47">
+        <f t="shared" si="0"/>
+        <v>1290.7104722792608</v>
+      </c>
+      <c r="N21" s="47">
+        <f t="shared" si="0"/>
+        <v>1288.7173169062287</v>
+      </c>
+      <c r="O21" s="47">
+        <f t="shared" si="0"/>
+        <v>1286.5817932922655</v>
+      </c>
+      <c r="P21" s="48">
+        <f t="shared" si="0"/>
+        <v>1284.3039014373717</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="49">
+        <f t="shared" ref="C22:P34" si="1">C6/365.25</f>
+        <v>1185.6427104722793</v>
+      </c>
+      <c r="D22" s="63">
+        <f t="shared" si="1"/>
+        <v>1190.4832306639289</v>
+      </c>
+      <c r="E22" s="63">
+        <f t="shared" si="1"/>
+        <v>1193.4729637234771</v>
+      </c>
+      <c r="F22" s="63">
+        <f t="shared" si="1"/>
+        <v>1194.8966461327857</v>
+      </c>
+      <c r="G22" s="63">
+        <f t="shared" si="1"/>
+        <v>1195.4661190965091</v>
+      </c>
+      <c r="H22" s="63">
+        <f t="shared" si="1"/>
+        <v>1195.3237508555783</v>
+      </c>
+      <c r="I22" s="63">
+        <f t="shared" si="1"/>
+        <v>1194.611909650924</v>
+      </c>
+      <c r="J22" s="63">
+        <f t="shared" si="1"/>
+        <v>1193.3305954825462</v>
+      </c>
+      <c r="K22" s="63">
+        <f t="shared" si="1"/>
+        <v>1191.6221765913758</v>
+      </c>
+      <c r="L22" s="63">
+        <f t="shared" si="1"/>
+        <v>1189.3442847364818</v>
+      </c>
+      <c r="M22" s="63">
+        <f t="shared" si="1"/>
+        <v>1186.4969199178645</v>
+      </c>
+      <c r="N22" s="63">
+        <f t="shared" si="1"/>
+        <v>1183.3648186173853</v>
+      </c>
+      <c r="O22" s="63">
+        <f t="shared" si="1"/>
+        <v>1179.8056125941137</v>
+      </c>
+      <c r="P22" s="51">
+        <f t="shared" si="1"/>
+        <v>1175.8193018480492</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="49">
+        <f t="shared" si="1"/>
+        <v>1036.4407939767282</v>
+      </c>
+      <c r="D23" s="63">
+        <f t="shared" si="1"/>
+        <v>1039.8576317590691</v>
+      </c>
+      <c r="E23" s="63">
+        <f t="shared" si="1"/>
+        <v>1041.7084188911704</v>
+      </c>
+      <c r="F23" s="63">
+        <f t="shared" si="1"/>
+        <v>1042.5626283367556</v>
+      </c>
+      <c r="G23" s="63">
+        <f t="shared" si="1"/>
+        <v>1042.8473648186173</v>
+      </c>
+      <c r="H23" s="63">
+        <f t="shared" si="1"/>
+        <v>1042.4202600958247</v>
+      </c>
+      <c r="I23" s="63">
+        <f t="shared" si="1"/>
+        <v>1041.5660506502395</v>
+      </c>
+      <c r="J23" s="63">
+        <f t="shared" si="1"/>
+        <v>1040.1423682409309</v>
+      </c>
+      <c r="K23" s="63">
+        <f t="shared" si="1"/>
+        <v>1038.2915811088296</v>
+      </c>
+      <c r="L23" s="63">
+        <f t="shared" si="1"/>
+        <v>1035.8713210130047</v>
+      </c>
+      <c r="M23" s="63">
+        <f t="shared" si="1"/>
+        <v>1032.8815879534566</v>
+      </c>
+      <c r="N23" s="63">
+        <f t="shared" si="1"/>
+        <v>1029.4647501711156</v>
+      </c>
+      <c r="O23" s="63">
+        <f t="shared" si="1"/>
+        <v>1025.7631759069131</v>
+      </c>
+      <c r="P23" s="51">
+        <f t="shared" si="1"/>
+        <v>1021.492128678987</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="49">
+        <f t="shared" si="1"/>
+        <v>1182.9377138945927</v>
+      </c>
+      <c r="D24" s="63">
+        <f t="shared" si="1"/>
+        <v>1187.3511293634497</v>
+      </c>
+      <c r="E24" s="63">
+        <f t="shared" si="1"/>
+        <v>1190.6255989048598</v>
+      </c>
+      <c r="F24" s="63">
+        <f t="shared" si="1"/>
+        <v>1192.7611225188227</v>
+      </c>
+      <c r="G24" s="63">
+        <f t="shared" si="1"/>
+        <v>1193.7577002053388</v>
+      </c>
+      <c r="H24" s="63">
+        <f t="shared" si="1"/>
+        <v>1194.0424366872005</v>
+      </c>
+      <c r="I24" s="63">
+        <f t="shared" si="1"/>
+        <v>1193.6153319644079</v>
+      </c>
+      <c r="J24" s="63">
+        <f t="shared" si="1"/>
+        <v>1192.7611225188227</v>
+      </c>
+      <c r="K24" s="63">
+        <f t="shared" si="1"/>
+        <v>1191.3374401095141</v>
+      </c>
+      <c r="L24" s="63">
+        <f t="shared" si="1"/>
+        <v>1189.3442847364818</v>
+      </c>
+      <c r="M24" s="63">
+        <f t="shared" si="1"/>
+        <v>1186.9240246406571</v>
+      </c>
+      <c r="N24" s="63">
+        <f t="shared" si="1"/>
+        <v>1184.0766598220398</v>
+      </c>
+      <c r="O24" s="63">
+        <f t="shared" si="1"/>
+        <v>1180.9445585215606</v>
+      </c>
+      <c r="P24" s="51">
+        <f t="shared" si="1"/>
+        <v>1177.5277207392196</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="49">
+        <f t="shared" si="1"/>
+        <v>1042.8473648186173</v>
+      </c>
+      <c r="D25" s="63">
+        <f t="shared" si="1"/>
+        <v>1047.1184120465434</v>
+      </c>
+      <c r="E25" s="63">
+        <f t="shared" si="1"/>
+        <v>1050.5352498288844</v>
+      </c>
+      <c r="F25" s="63">
+        <f t="shared" si="1"/>
+        <v>1052.9555099247091</v>
+      </c>
+      <c r="G25" s="63">
+        <f t="shared" si="1"/>
+        <v>1054.2368240930869</v>
+      </c>
+      <c r="H25" s="63">
+        <f t="shared" si="1"/>
+        <v>1054.6639288158794</v>
+      </c>
+      <c r="I25" s="63">
+        <f t="shared" si="1"/>
+        <v>1054.5215605749486</v>
+      </c>
+      <c r="J25" s="63">
+        <f t="shared" si="1"/>
+        <v>1054.094455852156</v>
+      </c>
+      <c r="K25" s="63">
+        <f t="shared" si="1"/>
+        <v>1053.0978781656399</v>
+      </c>
+      <c r="L25" s="63">
+        <f t="shared" si="1"/>
+        <v>1051.8165639972622</v>
+      </c>
+      <c r="M25" s="63">
+        <f t="shared" si="1"/>
+        <v>1050.2505133470227</v>
+      </c>
+      <c r="N25" s="63">
+        <f t="shared" si="1"/>
+        <v>1048.2573579739903</v>
+      </c>
+      <c r="O25" s="63">
+        <f t="shared" si="1"/>
+        <v>1045.9794661190965</v>
+      </c>
+      <c r="P25" s="51">
+        <f t="shared" si="1"/>
+        <v>1043.5592060232718</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="49">
+        <f t="shared" si="1"/>
+        <v>1257.3963039014375</v>
+      </c>
+      <c r="D26" s="63">
+        <f t="shared" si="1"/>
+        <v>1261.6673511293634</v>
+      </c>
+      <c r="E26" s="63">
+        <f t="shared" si="1"/>
+        <v>1264.7994524298426</v>
+      </c>
+      <c r="F26" s="63">
+        <f t="shared" si="1"/>
+        <v>1267.0773442847365</v>
+      </c>
+      <c r="G26" s="63">
+        <f t="shared" si="1"/>
+        <v>1268.3586584531142</v>
+      </c>
+      <c r="H26" s="63">
+        <f t="shared" si="1"/>
+        <v>1268.7857631759068</v>
+      </c>
+      <c r="I26" s="63">
+        <f t="shared" si="1"/>
+        <v>1268.7857631759068</v>
+      </c>
+      <c r="J26" s="63">
+        <f t="shared" si="1"/>
+        <v>1268.2162902121834</v>
+      </c>
+      <c r="K26" s="63">
+        <f t="shared" si="1"/>
+        <v>1267.0773442847365</v>
+      </c>
+      <c r="L26" s="63">
+        <f t="shared" si="1"/>
+        <v>1265.511293634497</v>
+      </c>
+      <c r="M26" s="63">
+        <f t="shared" si="1"/>
+        <v>1263.5181382614649</v>
+      </c>
+      <c r="N26" s="63">
+        <f t="shared" si="1"/>
+        <v>1261.0978781656399</v>
+      </c>
+      <c r="O26" s="63">
+        <f t="shared" si="1"/>
+        <v>1258.3928815879535</v>
+      </c>
+      <c r="P26" s="51">
+        <f t="shared" si="1"/>
+        <v>1255.4031485284052</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="49">
+        <f t="shared" si="1"/>
+        <v>1270.0670773442848</v>
+      </c>
+      <c r="D27" s="63">
+        <f t="shared" si="1"/>
+        <v>1273.7686516084873</v>
+      </c>
+      <c r="E27" s="63">
+        <f t="shared" si="1"/>
+        <v>1276.6160164271048</v>
+      </c>
+      <c r="F27" s="63">
+        <f t="shared" si="1"/>
+        <v>1278.466803559206</v>
+      </c>
+      <c r="G27" s="63">
+        <f t="shared" si="1"/>
+        <v>1279.6057494866529</v>
+      </c>
+      <c r="H27" s="63">
+        <f t="shared" si="1"/>
+        <v>1280.0328542094455</v>
+      </c>
+      <c r="I27" s="63">
+        <f t="shared" si="1"/>
+        <v>1279.8904859685147</v>
+      </c>
+      <c r="J27" s="63">
+        <f t="shared" si="1"/>
+        <v>1279.0362765229295</v>
+      </c>
+      <c r="K27" s="63">
+        <f t="shared" si="1"/>
+        <v>1277.6125941136208</v>
+      </c>
+      <c r="L27" s="63">
+        <f t="shared" si="1"/>
+        <v>1275.9041752224505</v>
+      </c>
+      <c r="M27" s="63">
+        <f t="shared" si="1"/>
+        <v>1273.4839151266256</v>
+      </c>
+      <c r="N27" s="63">
+        <f t="shared" si="1"/>
+        <v>1270.7789185489391</v>
+      </c>
+      <c r="O27" s="63">
+        <f t="shared" si="1"/>
+        <v>1267.504449007529</v>
+      </c>
+      <c r="P27" s="51">
+        <f t="shared" si="1"/>
+        <v>1263.9452429842574</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="49">
+        <f t="shared" si="1"/>
+        <v>1107.9096509240246</v>
+      </c>
+      <c r="D28" s="63">
+        <f t="shared" si="1"/>
+        <v>1112.1806981519508</v>
+      </c>
+      <c r="E28" s="63">
+        <f t="shared" si="1"/>
+        <v>1115.4551676933606</v>
+      </c>
+      <c r="F28" s="63">
+        <f t="shared" si="1"/>
+        <v>1117.5906913073238</v>
+      </c>
+      <c r="G28" s="63">
+        <f t="shared" si="1"/>
+        <v>1118.7296372347707</v>
+      </c>
+      <c r="H28" s="63">
+        <f t="shared" si="1"/>
+        <v>1119.1567419575633</v>
+      </c>
+      <c r="I28" s="63">
+        <f t="shared" si="1"/>
+        <v>1119.0143737166325</v>
+      </c>
+      <c r="J28" s="63">
+        <f t="shared" si="1"/>
+        <v>1118.444900752909</v>
+      </c>
+      <c r="K28" s="63">
+        <f t="shared" si="1"/>
+        <v>1117.448323066393</v>
+      </c>
+      <c r="L28" s="63">
+        <f t="shared" si="1"/>
+        <v>1116.0246406570841</v>
+      </c>
+      <c r="M28" s="63">
+        <f t="shared" si="1"/>
+        <v>1114.3162217659137</v>
+      </c>
+      <c r="N28" s="63">
+        <f t="shared" si="1"/>
+        <v>1112.3230663928816</v>
+      </c>
+      <c r="O28" s="63">
+        <f t="shared" si="1"/>
+        <v>1110.0451745379876</v>
+      </c>
+      <c r="P28" s="51">
+        <f t="shared" si="1"/>
+        <v>1107.482546201232</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="49">
+        <f t="shared" si="1"/>
+        <v>1207.9945242984256</v>
+      </c>
+      <c r="D29" s="63">
+        <f t="shared" si="1"/>
+        <v>1213.6892539356604</v>
+      </c>
+      <c r="E29" s="63">
+        <f t="shared" si="1"/>
+        <v>1218.1026694045174</v>
+      </c>
+      <c r="F29" s="63">
+        <f t="shared" si="1"/>
+        <v>1221.2347707049967</v>
+      </c>
+      <c r="G29" s="63">
+        <f t="shared" si="1"/>
+        <v>1223.5126625598905</v>
+      </c>
+      <c r="H29" s="63">
+        <f t="shared" si="1"/>
+        <v>1224.7939767282683</v>
+      </c>
+      <c r="I29" s="63">
+        <f t="shared" si="1"/>
+        <v>1225.3634496919917</v>
+      </c>
+      <c r="J29" s="63">
+        <f t="shared" si="1"/>
+        <v>1225.2210814510609</v>
+      </c>
+      <c r="K29" s="63">
+        <f t="shared" si="1"/>
+        <v>1224.3668720054757</v>
+      </c>
+      <c r="L29" s="63">
+        <f t="shared" si="1"/>
+        <v>1223.0855578370979</v>
+      </c>
+      <c r="M29" s="63">
+        <f t="shared" si="1"/>
+        <v>1220.8076659822041</v>
+      </c>
+      <c r="N29" s="63">
+        <f t="shared" si="1"/>
+        <v>1218.1026694045174</v>
+      </c>
+      <c r="O29" s="63">
+        <f t="shared" si="1"/>
+        <v>1214.5434633812458</v>
+      </c>
+      <c r="P29" s="51">
+        <f t="shared" si="1"/>
+        <v>1210.4147843942505</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="49">
+        <f t="shared" si="1"/>
+        <v>1233.4784394250514</v>
+      </c>
+      <c r="D30" s="63">
+        <f t="shared" si="1"/>
+        <v>1239.1731690622862</v>
+      </c>
+      <c r="E30" s="63">
+        <f t="shared" si="1"/>
+        <v>1241.8781656399726</v>
+      </c>
+      <c r="F30" s="63">
+        <f t="shared" si="1"/>
+        <v>1242.7323750855578</v>
+      </c>
+      <c r="G30" s="63">
+        <f t="shared" si="1"/>
+        <v>1243.0171115674195</v>
+      </c>
+      <c r="H30" s="63">
+        <f t="shared" si="1"/>
+        <v>1242.5900068446269</v>
+      </c>
+      <c r="I30" s="63">
+        <f t="shared" si="1"/>
+        <v>1241.7357973990418</v>
+      </c>
+      <c r="J30" s="63">
+        <f t="shared" si="1"/>
+        <v>1240.1697467488023</v>
+      </c>
+      <c r="K30" s="63">
+        <f t="shared" si="1"/>
+        <v>1238.0342231348391</v>
+      </c>
+      <c r="L30" s="63">
+        <f t="shared" si="1"/>
+        <v>1235.4715947980835</v>
+      </c>
+      <c r="M30" s="63">
+        <f t="shared" si="1"/>
+        <v>1232.4818617385351</v>
+      </c>
+      <c r="N30" s="63">
+        <f t="shared" si="1"/>
+        <v>1229.0650239561944</v>
+      </c>
+      <c r="O30" s="63">
+        <f t="shared" si="1"/>
+        <v>1225.07871321013</v>
+      </c>
+      <c r="P30" s="51">
+        <f t="shared" si="1"/>
+        <v>1220.6652977412732</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="49">
+        <f t="shared" si="1"/>
+        <v>1281.3141683778233</v>
+      </c>
+      <c r="D31" s="63">
+        <f t="shared" si="1"/>
+        <v>1285.7275838466803</v>
+      </c>
+      <c r="E31" s="63">
+        <f t="shared" si="1"/>
+        <v>1289.1444216290213</v>
+      </c>
+      <c r="F31" s="63">
+        <f t="shared" si="1"/>
+        <v>1291.564681724846</v>
+      </c>
+      <c r="G31" s="63">
+        <f t="shared" si="1"/>
+        <v>1293.1307323750855</v>
+      </c>
+      <c r="H31" s="63">
+        <f t="shared" si="1"/>
+        <v>1293.7002053388089</v>
+      </c>
+      <c r="I31" s="63">
+        <f t="shared" si="1"/>
+        <v>1293.5578370978781</v>
+      </c>
+      <c r="J31" s="63">
+        <f t="shared" si="1"/>
+        <v>1292.9883641341546</v>
+      </c>
+      <c r="K31" s="63">
+        <f t="shared" si="1"/>
+        <v>1291.9917864476386</v>
+      </c>
+      <c r="L31" s="63">
+        <f t="shared" si="1"/>
+        <v>1290.5681040383299</v>
+      </c>
+      <c r="M31" s="63">
+        <f t="shared" si="1"/>
+        <v>1288.8596851471596</v>
+      </c>
+      <c r="N31" s="63">
+        <f t="shared" si="1"/>
+        <v>1286.8665297741272</v>
+      </c>
+      <c r="O31" s="63">
+        <f t="shared" si="1"/>
+        <v>1284.4462696783025</v>
+      </c>
+      <c r="P31" s="51">
+        <f t="shared" si="1"/>
+        <v>1281.883641341547</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="49">
+        <f t="shared" si="1"/>
+        <v>1196.3203285420946</v>
+      </c>
+      <c r="D32" s="63">
+        <f t="shared" si="1"/>
+        <v>1203.7234770704997</v>
+      </c>
+      <c r="E32" s="63">
+        <f t="shared" si="1"/>
+        <v>1210.1300479123888</v>
+      </c>
+      <c r="F32" s="63">
+        <f t="shared" si="1"/>
+        <v>1215.6824093086927</v>
+      </c>
+      <c r="G32" s="63">
+        <f t="shared" si="1"/>
+        <v>1220.2381930184804</v>
+      </c>
+      <c r="H32" s="63">
+        <f t="shared" si="1"/>
+        <v>1223.9397672826831</v>
+      </c>
+      <c r="I32" s="63">
+        <f t="shared" si="1"/>
+        <v>1226.7871321013006</v>
+      </c>
+      <c r="J32" s="63">
+        <f t="shared" si="1"/>
+        <v>1229.0650239561944</v>
+      </c>
+      <c r="K32" s="63">
+        <f t="shared" si="1"/>
+        <v>1230.488706365503</v>
+      </c>
+      <c r="L32" s="63">
+        <f t="shared" si="1"/>
+        <v>1231.3429158110882</v>
+      </c>
+      <c r="M32" s="63">
+        <f t="shared" si="1"/>
+        <v>1231.7700205338808</v>
+      </c>
+      <c r="N32" s="63">
+        <f t="shared" si="1"/>
+        <v>1231.9123887748117</v>
+      </c>
+      <c r="O32" s="63">
+        <f t="shared" si="1"/>
+        <v>1231.7700205338808</v>
+      </c>
+      <c r="P32" s="51">
+        <f t="shared" si="1"/>
+        <v>1231.3429158110882</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="49">
+        <f t="shared" si="1"/>
+        <v>1385.3682683093771</v>
+      </c>
+      <c r="D33" s="63">
+        <f t="shared" si="1"/>
+        <v>1394.2625598904858</v>
+      </c>
+      <c r="E33" s="63">
+        <f t="shared" si="1"/>
+        <v>1401.8391786447639</v>
+      </c>
+      <c r="F33" s="63">
+        <f t="shared" si="1"/>
+        <v>1408.4275427789187</v>
+      </c>
+      <c r="G33" s="63">
+        <f t="shared" si="1"/>
+        <v>1414.0276522929501</v>
+      </c>
+      <c r="H33" s="63">
+        <f t="shared" si="1"/>
+        <v>1418.4747980835043</v>
+      </c>
+      <c r="I33" s="63">
+        <f t="shared" si="1"/>
+        <v>1422.0983983572896</v>
+      </c>
+      <c r="J33" s="63">
+        <f t="shared" si="1"/>
+        <v>1424.8984531143053</v>
+      </c>
+      <c r="K33" s="63">
+        <f t="shared" si="1"/>
+        <v>1426.7102532511979</v>
+      </c>
+      <c r="L33" s="63">
+        <f t="shared" si="1"/>
+        <v>1428.1926351813827</v>
+      </c>
+      <c r="M33" s="63">
+        <f t="shared" si="1"/>
+        <v>1429.1808898015058</v>
+      </c>
+      <c r="N33" s="63">
+        <f t="shared" si="1"/>
+        <v>1430.0044353182752</v>
+      </c>
+      <c r="O33" s="63">
+        <f t="shared" si="1"/>
+        <v>1430.4985626283369</v>
+      </c>
+      <c r="P33" s="51">
+        <f t="shared" si="1"/>
+        <v>1430.6632717316909</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="53">
+        <f t="shared" si="1"/>
+        <v>1229.2240383299109</v>
+      </c>
+      <c r="D34" s="54">
+        <f t="shared" si="1"/>
+        <v>1235.8124024640656</v>
+      </c>
+      <c r="E34" s="54">
+        <f t="shared" si="1"/>
+        <v>1240.9183846680355</v>
+      </c>
+      <c r="F34" s="54">
+        <f t="shared" si="1"/>
+        <v>1244.3772758384669</v>
+      </c>
+      <c r="G34" s="54">
+        <f t="shared" si="1"/>
+        <v>1246.5184941820671</v>
+      </c>
+      <c r="H34" s="54">
+        <f t="shared" si="1"/>
+        <v>1247.5067488021903</v>
+      </c>
+      <c r="I34" s="54">
+        <f t="shared" si="1"/>
+        <v>1247.8361670088982</v>
+      </c>
+      <c r="J34" s="54">
+        <f t="shared" si="1"/>
+        <v>1247.5067488021903</v>
+      </c>
+      <c r="K34" s="54">
+        <f t="shared" si="1"/>
+        <v>1246.1890759753594</v>
+      </c>
+      <c r="L34" s="54">
+        <f t="shared" si="1"/>
+        <v>1244.3772758384669</v>
+      </c>
+      <c r="M34" s="54">
+        <f t="shared" si="1"/>
+        <v>1241.7419301848051</v>
+      </c>
+      <c r="N34" s="54">
+        <f t="shared" si="1"/>
+        <v>1238.2830390143738</v>
+      </c>
+      <c r="O34" s="54">
+        <f t="shared" si="1"/>
+        <v>1233.8358932238195</v>
+      </c>
+      <c r="P34" s="55">
+        <f t="shared" si="1"/>
+        <v>1228.8946201232031</v>
       </c>
     </row>
   </sheetData>
@@ -9202,16 +10107,16 @@
       <selection activeCell="B2" sqref="B2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="45"/>
+      <c r="C2" s="62"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
@@ -10596,11 +11501,11 @@
         <v>96</v>
       </c>
       <c r="F100" s="1">
-        <f t="shared" ref="F100:F131" si="6">_xlfn.GAMMA.DIST(E100,$C$3,$C$4,0)</f>
+        <f t="shared" ref="F100:F104" si="6">_xlfn.GAMMA.DIST(E100,$C$3,$C$4,0)</f>
         <v>1.2866132713317674E-4</v>
       </c>
       <c r="G100" s="1">
-        <f t="shared" ref="G100:G131" si="7">_xlfn.GAMMA.INV(F100,$C$3,$C$4)</f>
+        <f t="shared" ref="G100:G104" si="7">_xlfn.GAMMA.INV(F100,$C$3,$C$4)</f>
         <v>1.8573616905076265</v>
       </c>
       <c r="K100" s="17"/>

</xml_diff>